<commit_message>
Removed personal info from excel files
</commit_message>
<xml_diff>
--- a/exampleSchedule.xlsx
+++ b/exampleSchedule.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <fileSharing readOnlyRecommended="1"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.hoopes\Documents\Local Backups\ScheduleTrak\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D6668C-DAF4-4123-BFA3-1BBE5D84AF1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9D6A65-6345-4442-BF0D-F7DE948DC911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="990" yWindow="-120" windowWidth="27930" windowHeight="16440" tabRatio="614" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -905,10 +900,40 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -919,16 +944,13 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -988,6 +1010,9 @@
     <xf numFmtId="0" fontId="8" fillId="18" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1000,6 +1025,9 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1008,39 +1036,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1535,14 +1530,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
+      <c r="A1" s="58"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1624,13 +1619,13 @@
       <c r="A5" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="60"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="69"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
     </row>
@@ -1638,15 +1633,15 @@
       <c r="A6" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="62"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="56" t="s">
+      <c r="C6" s="71"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="57"/>
+      <c r="F6" s="66"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
     </row>
@@ -1674,15 +1669,15 @@
       <c r="A8" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="65"/>
-      <c r="D8" s="66" t="s">
+      <c r="C8" s="74"/>
+      <c r="D8" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="67"/>
-      <c r="F8" s="68"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="77"/>
       <c r="G8" s="31"/>
       <c r="H8" s="31"/>
     </row>
@@ -1764,13 +1759,13 @@
       <c r="A12" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="69" t="s">
+      <c r="B12" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="71"/>
+      <c r="C12" s="79"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="80"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
@@ -1778,15 +1773,15 @@
       <c r="A13" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="61" t="s">
+      <c r="B13" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="62"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="56" t="s">
+      <c r="C13" s="71"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="57"/>
+      <c r="F13" s="66"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
@@ -1794,15 +1789,15 @@
       <c r="A14" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="57"/>
-      <c r="D14" s="73" t="s">
+      <c r="C14" s="66"/>
+      <c r="D14" s="82" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="82"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
@@ -1810,15 +1805,15 @@
       <c r="A15" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="64" t="s">
+      <c r="B15" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="65"/>
-      <c r="D15" s="72" t="s">
+      <c r="C15" s="74"/>
+      <c r="D15" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="72"/>
-      <c r="F15" s="72"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="81"/>
       <c r="G15" s="31"/>
       <c r="H15" s="31"/>
     </row>
@@ -1900,11 +1895,11 @@
       <c r="A19" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="61" t="s">
+      <c r="B19" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="62"/>
-      <c r="D19" s="74"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="83"/>
       <c r="E19" s="41" t="s">
         <v>35</v>
       </c>
@@ -1918,11 +1913,11 @@
       <c r="A20" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="61" t="s">
+      <c r="B20" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="62"/>
-      <c r="D20" s="63"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="72"/>
       <c r="E20" s="39" t="s">
         <v>35</v>
       </c>
@@ -1952,14 +1947,14 @@
       <c r="A22" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="64" t="s">
+      <c r="B22" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="65"/>
-      <c r="D22" s="75" t="s">
+      <c r="C22" s="74"/>
+      <c r="D22" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="76"/>
+      <c r="E22" s="86"/>
       <c r="F22" s="46" t="s">
         <v>34</v>
       </c>
@@ -2047,10 +2042,10 @@
       <c r="B26" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="77" t="s">
+      <c r="C26" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="71"/>
+      <c r="D26" s="80"/>
       <c r="E26" s="41" t="s">
         <v>38</v>
       </c>
@@ -2067,10 +2062,10 @@
       <c r="B27" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="77" t="s">
+      <c r="C27" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="71"/>
+      <c r="D27" s="80"/>
       <c r="E27" s="41" t="s">
         <v>38</v>
       </c>
@@ -2109,10 +2104,10 @@
       <c r="B29" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="75" t="s">
+      <c r="C29" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="76"/>
+      <c r="D29" s="86"/>
       <c r="E29" s="41" t="s">
         <v>38</v>
       </c>
@@ -2200,13 +2195,13 @@
       <c r="A33" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="49" t="s">
+      <c r="B33" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="50"/>
-      <c r="D33" s="50"/>
-      <c r="E33" s="50"/>
-      <c r="F33" s="51"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="61"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
     </row>
@@ -2214,13 +2209,13 @@
       <c r="A34" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="79" t="s">
+      <c r="B34" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="80"/>
-      <c r="D34" s="80"/>
-      <c r="E34" s="80"/>
-      <c r="F34" s="81"/>
+      <c r="C34" s="91"/>
+      <c r="D34" s="91"/>
+      <c r="E34" s="91"/>
+      <c r="F34" s="92"/>
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
     </row>
@@ -2237,10 +2232,10 @@
       <c r="D35" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E35" s="78" t="s">
+      <c r="E35" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="F35" s="51"/>
+      <c r="F35" s="61"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
     </row>
@@ -2248,13 +2243,13 @@
       <c r="A36" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="82" t="s">
+      <c r="B36" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="83"/>
-      <c r="D36" s="83"/>
-      <c r="E36" s="83"/>
-      <c r="F36" s="84"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="63"/>
+      <c r="E36" s="63"/>
+      <c r="F36" s="64"/>
       <c r="G36" s="31"/>
       <c r="H36" s="31"/>
     </row>
@@ -2336,15 +2331,15 @@
       <c r="A40" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B40" s="69" t="s">
+      <c r="B40" s="78" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="70"/>
-      <c r="D40" s="70"/>
-      <c r="E40" s="85" t="s">
+      <c r="C40" s="79"/>
+      <c r="D40" s="79"/>
+      <c r="E40" s="89" t="s">
         <v>47</v>
       </c>
-      <c r="F40" s="57"/>
+      <c r="F40" s="66"/>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
     </row>
@@ -2352,15 +2347,15 @@
       <c r="A41" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="69" t="s">
+      <c r="B41" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="70"/>
-      <c r="D41" s="70"/>
-      <c r="E41" s="77" t="s">
+      <c r="C41" s="79"/>
+      <c r="D41" s="79"/>
+      <c r="E41" s="87" t="s">
         <v>48</v>
       </c>
-      <c r="F41" s="71"/>
+      <c r="F41" s="80"/>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
     </row>
@@ -2368,15 +2363,15 @@
       <c r="A42" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="69" t="s">
+      <c r="B42" s="78" t="s">
         <v>46</v>
       </c>
-      <c r="C42" s="70"/>
-      <c r="D42" s="70"/>
-      <c r="E42" s="77" t="s">
+      <c r="C42" s="79"/>
+      <c r="D42" s="79"/>
+      <c r="E42" s="87" t="s">
         <v>49</v>
       </c>
-      <c r="F42" s="71"/>
+      <c r="F42" s="80"/>
       <c r="G42" s="13"/>
       <c r="H42" s="13"/>
     </row>
@@ -2384,19 +2379,19 @@
       <c r="A43" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B43" s="88" t="s">
+      <c r="B43" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="89" t="s">
+      <c r="C43" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="D43" s="89" t="s">
+      <c r="D43" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="E43" s="89" t="s">
+      <c r="E43" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="F43" s="90" t="s">
+      <c r="F43" s="51" t="s">
         <v>37</v>
       </c>
       <c r="G43" s="13"/>
@@ -2406,13 +2401,13 @@
       <c r="A44" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B44" s="91" t="s">
+      <c r="B44" s="84" t="s">
         <v>46</v>
       </c>
-      <c r="C44" s="91"/>
-      <c r="D44" s="91"/>
-      <c r="E44" s="92"/>
-      <c r="F44" s="92"/>
+      <c r="C44" s="84"/>
+      <c r="D44" s="84"/>
+      <c r="E44" s="52"/>
+      <c r="F44" s="52"/>
       <c r="G44" s="31"/>
       <c r="H44" s="31"/>
     </row>
@@ -2452,41 +2447,41 @@
     </row>
     <row r="47" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="23"/>
-      <c r="B47" s="86"/>
-      <c r="C47" s="86"/>
-      <c r="D47" s="86"/>
-      <c r="E47" s="86"/>
-      <c r="F47" s="86"/>
+      <c r="B47" s="47"/>
+      <c r="C47" s="47"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="47"/>
+      <c r="F47" s="47"/>
       <c r="G47" s="22"/>
       <c r="H47" s="22"/>
     </row>
     <row r="48" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="23"/>
-      <c r="B48" s="87"/>
-      <c r="C48" s="87"/>
-      <c r="D48" s="87"/>
-      <c r="E48" s="87"/>
-      <c r="F48" s="87"/>
+      <c r="B48" s="48"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="48"/>
+      <c r="E48" s="48"/>
+      <c r="F48" s="48"/>
       <c r="G48" s="22"/>
       <c r="H48" s="22"/>
     </row>
     <row r="49" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="23"/>
-      <c r="B49" s="87"/>
-      <c r="C49" s="87"/>
-      <c r="D49" s="87"/>
-      <c r="E49" s="87"/>
-      <c r="F49" s="87"/>
+      <c r="B49" s="48"/>
+      <c r="C49" s="48"/>
+      <c r="D49" s="48"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="48"/>
       <c r="G49" s="22"/>
       <c r="H49" s="22"/>
     </row>
     <row r="50" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="18"/>
-      <c r="B50" s="86"/>
-      <c r="C50" s="86"/>
-      <c r="D50" s="86"/>
-      <c r="E50" s="86"/>
-      <c r="F50" s="86"/>
+      <c r="B50" s="47"/>
+      <c r="C50" s="47"/>
+      <c r="D50" s="47"/>
+      <c r="E50" s="47"/>
+      <c r="F50" s="47"/>
       <c r="G50" s="22"/>
       <c r="H50" s="22"/>
     </row>
@@ -2502,11 +2497,11 @@
     </row>
     <row r="52" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="18"/>
-      <c r="B52" s="47"/>
-      <c r="C52" s="47"/>
-      <c r="D52" s="47"/>
-      <c r="E52" s="47"/>
-      <c r="F52" s="47"/>
+      <c r="B52" s="55"/>
+      <c r="C52" s="55"/>
+      <c r="D52" s="55"/>
+      <c r="E52" s="55"/>
+      <c r="F52" s="55"/>
       <c r="G52" s="22"/>
       <c r="H52" s="22"/>
     </row>
@@ -2532,11 +2527,11 @@
     </row>
     <row r="55" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="23"/>
-      <c r="B55" s="48"/>
-      <c r="C55" s="48"/>
-      <c r="D55" s="48"/>
-      <c r="E55" s="48"/>
-      <c r="F55" s="48"/>
+      <c r="B55" s="56"/>
+      <c r="C55" s="56"/>
+      <c r="D55" s="56"/>
+      <c r="E55" s="56"/>
+      <c r="F55" s="56"/>
       <c r="G55" s="22"/>
       <c r="H55" s="22"/>
     </row>
@@ -2582,11 +2577,11 @@
     </row>
     <row r="60" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="23"/>
-      <c r="B60" s="52"/>
-      <c r="C60" s="52"/>
-      <c r="D60" s="52"/>
-      <c r="E60" s="52"/>
-      <c r="F60" s="52"/>
+      <c r="B60" s="54"/>
+      <c r="C60" s="54"/>
+      <c r="D60" s="54"/>
+      <c r="E60" s="54"/>
+      <c r="F60" s="54"/>
       <c r="G60" s="22"/>
       <c r="H60" s="22"/>
     </row>
@@ -2612,11 +2607,11 @@
     </row>
     <row r="63" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="18"/>
-      <c r="B63" s="52"/>
-      <c r="C63" s="52"/>
-      <c r="D63" s="52"/>
-      <c r="E63" s="52"/>
-      <c r="F63" s="52"/>
+      <c r="B63" s="54"/>
+      <c r="C63" s="54"/>
+      <c r="D63" s="54"/>
+      <c r="E63" s="54"/>
+      <c r="F63" s="54"/>
       <c r="G63" s="22"/>
       <c r="H63" s="22"/>
     </row>
@@ -2633,20 +2628,20 @@
     <row r="65" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="18"/>
       <c r="B65" s="21"/>
-      <c r="C65" s="47"/>
-      <c r="D65" s="47"/>
-      <c r="E65" s="47"/>
-      <c r="F65" s="47"/>
+      <c r="C65" s="55"/>
+      <c r="D65" s="55"/>
+      <c r="E65" s="55"/>
+      <c r="F65" s="55"/>
       <c r="G65" s="22"/>
       <c r="H65" s="22"/>
     </row>
     <row r="66" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="18"/>
-      <c r="B66" s="47"/>
-      <c r="C66" s="47"/>
-      <c r="D66" s="47"/>
-      <c r="E66" s="47"/>
-      <c r="F66" s="47"/>
+      <c r="B66" s="55"/>
+      <c r="C66" s="55"/>
+      <c r="D66" s="55"/>
+      <c r="E66" s="55"/>
+      <c r="F66" s="55"/>
       <c r="G66" s="22"/>
       <c r="H66" s="22"/>
     </row>
@@ -2662,11 +2657,11 @@
     </row>
     <row r="68" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="23"/>
-      <c r="B68" s="48"/>
-      <c r="C68" s="48"/>
-      <c r="D68" s="48"/>
-      <c r="E68" s="48"/>
-      <c r="F68" s="48"/>
+      <c r="B68" s="56"/>
+      <c r="C68" s="56"/>
+      <c r="D68" s="56"/>
+      <c r="E68" s="56"/>
+      <c r="F68" s="56"/>
       <c r="G68" s="22"/>
       <c r="H68" s="22"/>
     </row>
@@ -2712,11 +2707,11 @@
     </row>
     <row r="73" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="23"/>
-      <c r="B73" s="52"/>
-      <c r="C73" s="52"/>
-      <c r="D73" s="52"/>
-      <c r="E73" s="52"/>
-      <c r="F73" s="52"/>
+      <c r="B73" s="54"/>
+      <c r="C73" s="54"/>
+      <c r="D73" s="54"/>
+      <c r="E73" s="54"/>
+      <c r="F73" s="54"/>
       <c r="G73" s="22"/>
       <c r="H73" s="22"/>
     </row>
@@ -2742,11 +2737,11 @@
     </row>
     <row r="76" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="18"/>
-      <c r="B76" s="52"/>
-      <c r="C76" s="52"/>
-      <c r="D76" s="52"/>
-      <c r="E76" s="52"/>
-      <c r="F76" s="52"/>
+      <c r="B76" s="54"/>
+      <c r="C76" s="54"/>
+      <c r="D76" s="54"/>
+      <c r="E76" s="54"/>
+      <c r="F76" s="54"/>
       <c r="G76" s="22"/>
       <c r="H76" s="22"/>
     </row>
@@ -2762,21 +2757,21 @@
     </row>
     <row r="78" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="18"/>
-      <c r="B78" s="47"/>
-      <c r="C78" s="47"/>
-      <c r="D78" s="47"/>
-      <c r="E78" s="47"/>
-      <c r="F78" s="47"/>
+      <c r="B78" s="55"/>
+      <c r="C78" s="55"/>
+      <c r="D78" s="55"/>
+      <c r="E78" s="55"/>
+      <c r="F78" s="55"/>
       <c r="G78" s="22"/>
       <c r="H78" s="22"/>
     </row>
     <row r="79" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="18"/>
-      <c r="B79" s="47"/>
-      <c r="C79" s="47"/>
-      <c r="D79" s="47"/>
-      <c r="E79" s="47"/>
-      <c r="F79" s="47"/>
+      <c r="B79" s="55"/>
+      <c r="C79" s="55"/>
+      <c r="D79" s="55"/>
+      <c r="E79" s="55"/>
+      <c r="F79" s="55"/>
       <c r="G79" s="22"/>
       <c r="H79" s="22"/>
     </row>
@@ -2792,11 +2787,11 @@
     </row>
     <row r="81" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="23"/>
-      <c r="B81" s="48"/>
-      <c r="C81" s="48"/>
-      <c r="D81" s="48"/>
-      <c r="E81" s="48"/>
-      <c r="F81" s="48"/>
+      <c r="B81" s="56"/>
+      <c r="C81" s="56"/>
+      <c r="D81" s="56"/>
+      <c r="E81" s="56"/>
+      <c r="F81" s="56"/>
       <c r="G81" s="22"/>
       <c r="H81" s="22"/>
     </row>
@@ -2842,11 +2837,11 @@
     </row>
     <row r="86" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="23"/>
-      <c r="B86" s="47"/>
-      <c r="C86" s="47"/>
-      <c r="D86" s="47"/>
-      <c r="E86" s="47"/>
-      <c r="F86" s="47"/>
+      <c r="B86" s="55"/>
+      <c r="C86" s="55"/>
+      <c r="D86" s="55"/>
+      <c r="E86" s="55"/>
+      <c r="F86" s="55"/>
       <c r="G86" s="22"/>
       <c r="H86" s="22"/>
     </row>
@@ -2872,19 +2867,19 @@
     </row>
     <row r="89" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="18"/>
-      <c r="B89" s="47"/>
-      <c r="C89" s="47"/>
-      <c r="D89" s="47"/>
-      <c r="E89" s="47"/>
-      <c r="F89" s="47"/>
+      <c r="B89" s="55"/>
+      <c r="C89" s="55"/>
+      <c r="D89" s="55"/>
+      <c r="E89" s="55"/>
+      <c r="F89" s="55"/>
       <c r="G89" s="22"/>
       <c r="H89" s="22"/>
     </row>
     <row r="90" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="23"/>
-      <c r="B90" s="47"/>
-      <c r="C90" s="47"/>
-      <c r="D90" s="47"/>
+      <c r="B90" s="55"/>
+      <c r="C90" s="55"/>
+      <c r="D90" s="55"/>
       <c r="E90" s="21"/>
       <c r="F90" s="21"/>
       <c r="G90" s="22"/>
@@ -2902,11 +2897,11 @@
     </row>
     <row r="92" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="18"/>
-      <c r="B92" s="47"/>
-      <c r="C92" s="47"/>
-      <c r="D92" s="47"/>
-      <c r="E92" s="47"/>
-      <c r="F92" s="47"/>
+      <c r="B92" s="55"/>
+      <c r="C92" s="55"/>
+      <c r="D92" s="55"/>
+      <c r="E92" s="55"/>
+      <c r="F92" s="55"/>
       <c r="G92" s="22"/>
       <c r="H92" s="22"/>
     </row>
@@ -2922,11 +2917,11 @@
     </row>
     <row r="94" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="23"/>
-      <c r="B94" s="48"/>
-      <c r="C94" s="48"/>
-      <c r="D94" s="48"/>
-      <c r="E94" s="48"/>
-      <c r="F94" s="48"/>
+      <c r="B94" s="56"/>
+      <c r="C94" s="56"/>
+      <c r="D94" s="56"/>
+      <c r="E94" s="56"/>
+      <c r="F94" s="56"/>
       <c r="G94" s="22"/>
       <c r="H94" s="22"/>
     </row>
@@ -2972,11 +2967,11 @@
     </row>
     <row r="99" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="23"/>
-      <c r="B99" s="47"/>
-      <c r="C99" s="47"/>
-      <c r="D99" s="47"/>
-      <c r="E99" s="47"/>
-      <c r="F99" s="47"/>
+      <c r="B99" s="55"/>
+      <c r="C99" s="55"/>
+      <c r="D99" s="55"/>
+      <c r="E99" s="55"/>
+      <c r="F99" s="55"/>
       <c r="G99" s="22"/>
       <c r="H99" s="22"/>
     </row>
@@ -3002,11 +2997,11 @@
     </row>
     <row r="102" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="18"/>
-      <c r="B102" s="47"/>
-      <c r="C102" s="47"/>
-      <c r="D102" s="47"/>
-      <c r="E102" s="47"/>
-      <c r="F102" s="47"/>
+      <c r="B102" s="55"/>
+      <c r="C102" s="55"/>
+      <c r="D102" s="55"/>
+      <c r="E102" s="55"/>
+      <c r="F102" s="55"/>
       <c r="G102" s="22"/>
       <c r="H102" s="22"/>
     </row>
@@ -3052,11 +3047,11 @@
     </row>
     <row r="107" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="23"/>
-      <c r="B107" s="48"/>
-      <c r="C107" s="48"/>
-      <c r="D107" s="48"/>
-      <c r="E107" s="48"/>
-      <c r="F107" s="48"/>
+      <c r="B107" s="56"/>
+      <c r="C107" s="56"/>
+      <c r="D107" s="56"/>
+      <c r="E107" s="56"/>
+      <c r="F107" s="56"/>
       <c r="G107" s="22"/>
       <c r="H107" s="22"/>
     </row>
@@ -3102,11 +3097,11 @@
     </row>
     <row r="112" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="23"/>
-      <c r="B112" s="47"/>
-      <c r="C112" s="47"/>
-      <c r="D112" s="47"/>
-      <c r="E112" s="47"/>
-      <c r="F112" s="47"/>
+      <c r="B112" s="55"/>
+      <c r="C112" s="55"/>
+      <c r="D112" s="55"/>
+      <c r="E112" s="55"/>
+      <c r="F112" s="55"/>
       <c r="G112" s="22"/>
       <c r="H112" s="22"/>
     </row>
@@ -3132,11 +3127,11 @@
     </row>
     <row r="115" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="18"/>
-      <c r="B115" s="47"/>
-      <c r="C115" s="47"/>
-      <c r="D115" s="47"/>
-      <c r="E115" s="47"/>
-      <c r="F115" s="47"/>
+      <c r="B115" s="55"/>
+      <c r="C115" s="55"/>
+      <c r="D115" s="55"/>
+      <c r="E115" s="55"/>
+      <c r="F115" s="55"/>
       <c r="G115" s="22"/>
       <c r="H115" s="22"/>
     </row>
@@ -3182,11 +3177,11 @@
     </row>
     <row r="120" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="23"/>
-      <c r="B120" s="48"/>
-      <c r="C120" s="48"/>
-      <c r="D120" s="48"/>
-      <c r="E120" s="48"/>
-      <c r="F120" s="48"/>
+      <c r="B120" s="56"/>
+      <c r="C120" s="56"/>
+      <c r="D120" s="56"/>
+      <c r="E120" s="56"/>
+      <c r="F120" s="56"/>
       <c r="G120" s="22"/>
       <c r="H120" s="22"/>
     </row>
@@ -3232,11 +3227,11 @@
     </row>
     <row r="125" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="23"/>
-      <c r="B125" s="47"/>
-      <c r="C125" s="47"/>
-      <c r="D125" s="47"/>
-      <c r="E125" s="47"/>
-      <c r="F125" s="47"/>
+      <c r="B125" s="55"/>
+      <c r="C125" s="55"/>
+      <c r="D125" s="55"/>
+      <c r="E125" s="55"/>
+      <c r="F125" s="55"/>
       <c r="G125" s="22"/>
       <c r="H125" s="22"/>
     </row>
@@ -3252,21 +3247,21 @@
     </row>
     <row r="127" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="23"/>
-      <c r="B127" s="47"/>
-      <c r="C127" s="47"/>
-      <c r="D127" s="47"/>
-      <c r="E127" s="47"/>
-      <c r="F127" s="47"/>
+      <c r="B127" s="55"/>
+      <c r="C127" s="55"/>
+      <c r="D127" s="55"/>
+      <c r="E127" s="55"/>
+      <c r="F127" s="55"/>
       <c r="G127" s="22"/>
       <c r="H127" s="22"/>
     </row>
     <row r="128" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="18"/>
-      <c r="B128" s="47"/>
-      <c r="C128" s="47"/>
-      <c r="D128" s="47"/>
-      <c r="E128" s="47"/>
-      <c r="F128" s="47"/>
+      <c r="B128" s="55"/>
+      <c r="C128" s="55"/>
+      <c r="D128" s="55"/>
+      <c r="E128" s="55"/>
+      <c r="F128" s="55"/>
       <c r="G128" s="22"/>
       <c r="H128" s="22"/>
     </row>
@@ -3292,11 +3287,11 @@
     </row>
     <row r="131" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="18"/>
-      <c r="B131" s="47"/>
-      <c r="C131" s="47"/>
-      <c r="D131" s="47"/>
-      <c r="E131" s="47"/>
-      <c r="F131" s="47"/>
+      <c r="B131" s="55"/>
+      <c r="C131" s="55"/>
+      <c r="D131" s="55"/>
+      <c r="E131" s="55"/>
+      <c r="F131" s="55"/>
       <c r="G131" s="22"/>
       <c r="H131" s="22"/>
     </row>
@@ -3312,11 +3307,11 @@
     </row>
     <row r="133" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="23"/>
-      <c r="B133" s="48"/>
-      <c r="C133" s="48"/>
-      <c r="D133" s="48"/>
-      <c r="E133" s="48"/>
-      <c r="F133" s="48"/>
+      <c r="B133" s="56"/>
+      <c r="C133" s="56"/>
+      <c r="D133" s="56"/>
+      <c r="E133" s="56"/>
+      <c r="F133" s="56"/>
       <c r="G133" s="22"/>
       <c r="H133" s="22"/>
     </row>
@@ -3362,11 +3357,11 @@
     </row>
     <row r="138" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="23"/>
-      <c r="B138" s="47"/>
-      <c r="C138" s="47"/>
-      <c r="D138" s="47"/>
-      <c r="E138" s="47"/>
-      <c r="F138" s="47"/>
+      <c r="B138" s="55"/>
+      <c r="C138" s="55"/>
+      <c r="D138" s="55"/>
+      <c r="E138" s="55"/>
+      <c r="F138" s="55"/>
       <c r="G138" s="22"/>
       <c r="H138" s="22"/>
     </row>
@@ -3382,21 +3377,21 @@
     </row>
     <row r="140" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="23"/>
-      <c r="B140" s="47"/>
-      <c r="C140" s="47"/>
-      <c r="D140" s="47"/>
-      <c r="E140" s="47"/>
-      <c r="F140" s="47"/>
+      <c r="B140" s="55"/>
+      <c r="C140" s="55"/>
+      <c r="D140" s="55"/>
+      <c r="E140" s="55"/>
+      <c r="F140" s="55"/>
       <c r="G140" s="22"/>
       <c r="H140" s="22"/>
     </row>
     <row r="141" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="18"/>
-      <c r="B141" s="47"/>
-      <c r="C141" s="47"/>
-      <c r="D141" s="47"/>
-      <c r="E141" s="47"/>
-      <c r="F141" s="47"/>
+      <c r="B141" s="55"/>
+      <c r="C141" s="55"/>
+      <c r="D141" s="55"/>
+      <c r="E141" s="55"/>
+      <c r="F141" s="55"/>
       <c r="G141" s="22"/>
       <c r="H141" s="22"/>
     </row>
@@ -3412,51 +3407,51 @@
     </row>
     <row r="143" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="18"/>
-      <c r="B143" s="47"/>
-      <c r="C143" s="47"/>
-      <c r="D143" s="47"/>
-      <c r="E143" s="47"/>
-      <c r="F143" s="47"/>
+      <c r="B143" s="55"/>
+      <c r="C143" s="55"/>
+      <c r="D143" s="55"/>
+      <c r="E143" s="55"/>
+      <c r="F143" s="55"/>
       <c r="G143" s="22"/>
       <c r="H143" s="22"/>
     </row>
     <row r="144" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="18"/>
-      <c r="B144" s="47"/>
-      <c r="C144" s="47"/>
-      <c r="D144" s="47"/>
-      <c r="E144" s="47"/>
-      <c r="F144" s="47"/>
+      <c r="B144" s="55"/>
+      <c r="C144" s="55"/>
+      <c r="D144" s="55"/>
+      <c r="E144" s="55"/>
+      <c r="F144" s="55"/>
       <c r="G144" s="22"/>
       <c r="H144" s="22"/>
     </row>
     <row r="145" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="18"/>
-      <c r="B145" s="47"/>
-      <c r="C145" s="47"/>
-      <c r="D145" s="47"/>
-      <c r="E145" s="47"/>
-      <c r="F145" s="47"/>
+      <c r="B145" s="55"/>
+      <c r="C145" s="55"/>
+      <c r="D145" s="55"/>
+      <c r="E145" s="55"/>
+      <c r="F145" s="55"/>
       <c r="G145" s="22"/>
       <c r="H145" s="22"/>
     </row>
     <row r="146" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="18"/>
-      <c r="B146" s="47"/>
-      <c r="C146" s="47"/>
-      <c r="D146" s="47"/>
-      <c r="E146" s="47"/>
-      <c r="F146" s="47"/>
+      <c r="B146" s="55"/>
+      <c r="C146" s="55"/>
+      <c r="D146" s="55"/>
+      <c r="E146" s="55"/>
+      <c r="F146" s="55"/>
       <c r="G146" s="22"/>
       <c r="H146" s="22"/>
     </row>
     <row r="147" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="18"/>
-      <c r="B147" s="47"/>
-      <c r="C147" s="47"/>
-      <c r="D147" s="47"/>
-      <c r="E147" s="47"/>
-      <c r="F147" s="47"/>
+      <c r="B147" s="55"/>
+      <c r="C147" s="55"/>
+      <c r="D147" s="55"/>
+      <c r="E147" s="55"/>
+      <c r="F147" s="55"/>
       <c r="G147" s="22"/>
       <c r="H147" s="22"/>
     </row>
@@ -3472,11 +3467,11 @@
     </row>
     <row r="149" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="23"/>
-      <c r="B149" s="48"/>
-      <c r="C149" s="48"/>
-      <c r="D149" s="48"/>
-      <c r="E149" s="48"/>
-      <c r="F149" s="48"/>
+      <c r="B149" s="56"/>
+      <c r="C149" s="56"/>
+      <c r="D149" s="56"/>
+      <c r="E149" s="56"/>
+      <c r="F149" s="56"/>
       <c r="G149" s="22"/>
       <c r="H149" s="22"/>
     </row>
@@ -3522,10 +3517,10 @@
     </row>
     <row r="154" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="23"/>
-      <c r="B154" s="47"/>
-      <c r="C154" s="47"/>
-      <c r="D154" s="47"/>
-      <c r="E154" s="47"/>
+      <c r="B154" s="55"/>
+      <c r="C154" s="55"/>
+      <c r="D154" s="55"/>
+      <c r="E154" s="55"/>
       <c r="F154" s="21"/>
       <c r="G154" s="22"/>
       <c r="H154" s="22"/>
@@ -3552,10 +3547,10 @@
     </row>
     <row r="157" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="18"/>
-      <c r="B157" s="47"/>
-      <c r="C157" s="47"/>
-      <c r="D157" s="47"/>
-      <c r="E157" s="47"/>
+      <c r="B157" s="55"/>
+      <c r="C157" s="55"/>
+      <c r="D157" s="55"/>
+      <c r="E157" s="55"/>
       <c r="F157" s="21"/>
       <c r="G157" s="22"/>
       <c r="H157" s="22"/>
@@ -3572,60 +3567,60 @@
     </row>
     <row r="159" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="18"/>
-      <c r="B159" s="47"/>
-      <c r="C159" s="47"/>
-      <c r="D159" s="47"/>
-      <c r="E159" s="47"/>
+      <c r="B159" s="55"/>
+      <c r="C159" s="55"/>
+      <c r="D159" s="55"/>
+      <c r="E159" s="55"/>
       <c r="F159" s="21"/>
       <c r="G159" s="22"/>
       <c r="H159" s="22"/>
     </row>
     <row r="160" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="27"/>
-      <c r="B160" s="47"/>
-      <c r="C160" s="47"/>
-      <c r="D160" s="47"/>
-      <c r="E160" s="47"/>
+      <c r="B160" s="55"/>
+      <c r="C160" s="55"/>
+      <c r="D160" s="55"/>
+      <c r="E160" s="55"/>
       <c r="F160" s="21"/>
       <c r="G160" s="21"/>
       <c r="H160" s="21"/>
     </row>
     <row r="161" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="18"/>
-      <c r="B161" s="47"/>
-      <c r="C161" s="47"/>
-      <c r="D161" s="47"/>
-      <c r="E161" s="47"/>
+      <c r="B161" s="55"/>
+      <c r="C161" s="55"/>
+      <c r="D161" s="55"/>
+      <c r="E161" s="55"/>
       <c r="F161" s="21"/>
       <c r="G161" s="21"/>
       <c r="H161" s="21"/>
     </row>
     <row r="162" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="18"/>
-      <c r="B162" s="47"/>
-      <c r="C162" s="47"/>
-      <c r="D162" s="47"/>
-      <c r="E162" s="47"/>
+      <c r="B162" s="55"/>
+      <c r="C162" s="55"/>
+      <c r="D162" s="55"/>
+      <c r="E162" s="55"/>
       <c r="F162" s="21"/>
       <c r="G162" s="22"/>
       <c r="H162" s="22"/>
     </row>
     <row r="163" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="27"/>
-      <c r="B163" s="47"/>
-      <c r="C163" s="47"/>
-      <c r="D163" s="47"/>
-      <c r="E163" s="47"/>
+      <c r="B163" s="55"/>
+      <c r="C163" s="55"/>
+      <c r="D163" s="55"/>
+      <c r="E163" s="55"/>
       <c r="F163" s="21"/>
       <c r="G163" s="21"/>
       <c r="H163" s="21"/>
     </row>
     <row r="164" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="18"/>
-      <c r="B164" s="47"/>
-      <c r="C164" s="47"/>
-      <c r="D164" s="47"/>
-      <c r="E164" s="47"/>
+      <c r="B164" s="55"/>
+      <c r="C164" s="55"/>
+      <c r="D164" s="55"/>
+      <c r="E164" s="55"/>
       <c r="F164" s="21"/>
       <c r="G164" s="21"/>
       <c r="H164" s="21"/>
@@ -3642,10 +3637,10 @@
     </row>
     <row r="166" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="23"/>
-      <c r="B166" s="48"/>
-      <c r="C166" s="48"/>
-      <c r="D166" s="48"/>
-      <c r="E166" s="48"/>
+      <c r="B166" s="56"/>
+      <c r="C166" s="56"/>
+      <c r="D166" s="56"/>
+      <c r="E166" s="56"/>
       <c r="F166" s="28"/>
       <c r="G166" s="22"/>
       <c r="H166" s="22"/>
@@ -3692,21 +3687,21 @@
     </row>
     <row r="171" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="23"/>
-      <c r="B171" s="47"/>
-      <c r="C171" s="47"/>
-      <c r="D171" s="47"/>
-      <c r="E171" s="47"/>
-      <c r="F171" s="47"/>
+      <c r="B171" s="55"/>
+      <c r="C171" s="55"/>
+      <c r="D171" s="55"/>
+      <c r="E171" s="55"/>
+      <c r="F171" s="55"/>
       <c r="G171" s="22"/>
       <c r="H171" s="22"/>
     </row>
     <row r="172" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="23"/>
-      <c r="B172" s="47"/>
-      <c r="C172" s="47"/>
-      <c r="D172" s="47"/>
-      <c r="E172" s="47"/>
-      <c r="F172" s="47"/>
+      <c r="B172" s="55"/>
+      <c r="C172" s="55"/>
+      <c r="D172" s="55"/>
+      <c r="E172" s="55"/>
+      <c r="F172" s="55"/>
       <c r="G172" s="22"/>
       <c r="H172" s="22"/>
     </row>
@@ -3722,11 +3717,11 @@
     </row>
     <row r="174" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="18"/>
-      <c r="B174" s="47"/>
-      <c r="C174" s="47"/>
-      <c r="D174" s="47"/>
-      <c r="E174" s="47"/>
-      <c r="F174" s="47"/>
+      <c r="B174" s="55"/>
+      <c r="C174" s="55"/>
+      <c r="D174" s="55"/>
+      <c r="E174" s="55"/>
+      <c r="F174" s="55"/>
       <c r="G174" s="22"/>
       <c r="H174" s="22"/>
     </row>
@@ -3742,61 +3737,61 @@
     </row>
     <row r="176" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="18"/>
-      <c r="B176" s="47"/>
-      <c r="C176" s="47"/>
-      <c r="D176" s="47"/>
-      <c r="E176" s="47"/>
-      <c r="F176" s="47"/>
+      <c r="B176" s="55"/>
+      <c r="C176" s="55"/>
+      <c r="D176" s="55"/>
+      <c r="E176" s="55"/>
+      <c r="F176" s="55"/>
       <c r="G176" s="22"/>
       <c r="H176" s="22"/>
     </row>
     <row r="177" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="18"/>
-      <c r="B177" s="47"/>
-      <c r="C177" s="47"/>
-      <c r="D177" s="47"/>
-      <c r="E177" s="47"/>
-      <c r="F177" s="47"/>
+      <c r="B177" s="55"/>
+      <c r="C177" s="55"/>
+      <c r="D177" s="55"/>
+      <c r="E177" s="55"/>
+      <c r="F177" s="55"/>
       <c r="G177" s="22"/>
       <c r="H177" s="22"/>
     </row>
     <row r="178" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="18"/>
-      <c r="B178" s="47"/>
-      <c r="C178" s="47"/>
-      <c r="D178" s="47"/>
-      <c r="E178" s="47"/>
-      <c r="F178" s="47"/>
+      <c r="B178" s="55"/>
+      <c r="C178" s="55"/>
+      <c r="D178" s="55"/>
+      <c r="E178" s="55"/>
+      <c r="F178" s="55"/>
       <c r="G178" s="22"/>
       <c r="H178" s="22"/>
     </row>
     <row r="179" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="18"/>
-      <c r="B179" s="47"/>
-      <c r="C179" s="47"/>
-      <c r="D179" s="47"/>
-      <c r="E179" s="47"/>
-      <c r="F179" s="47"/>
+      <c r="B179" s="55"/>
+      <c r="C179" s="55"/>
+      <c r="D179" s="55"/>
+      <c r="E179" s="55"/>
+      <c r="F179" s="55"/>
       <c r="G179" s="22"/>
       <c r="H179" s="22"/>
     </row>
     <row r="180" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="18"/>
-      <c r="B180" s="47"/>
-      <c r="C180" s="47"/>
-      <c r="D180" s="47"/>
-      <c r="E180" s="47"/>
-      <c r="F180" s="47"/>
+      <c r="B180" s="55"/>
+      <c r="C180" s="55"/>
+      <c r="D180" s="55"/>
+      <c r="E180" s="55"/>
+      <c r="F180" s="55"/>
       <c r="G180" s="22"/>
       <c r="H180" s="22"/>
     </row>
     <row r="181" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="18"/>
-      <c r="B181" s="47"/>
-      <c r="C181" s="47"/>
-      <c r="D181" s="47"/>
-      <c r="E181" s="47"/>
-      <c r="F181" s="47"/>
+      <c r="B181" s="55"/>
+      <c r="C181" s="55"/>
+      <c r="D181" s="55"/>
+      <c r="E181" s="55"/>
+      <c r="F181" s="55"/>
       <c r="G181" s="22"/>
       <c r="H181" s="22"/>
     </row>
@@ -3812,11 +3807,11 @@
     </row>
     <row r="183" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="23"/>
-      <c r="B183" s="48"/>
-      <c r="C183" s="48"/>
-      <c r="D183" s="48"/>
-      <c r="E183" s="48"/>
-      <c r="F183" s="48"/>
+      <c r="B183" s="56"/>
+      <c r="C183" s="56"/>
+      <c r="D183" s="56"/>
+      <c r="E183" s="56"/>
+      <c r="F183" s="56"/>
       <c r="G183" s="22"/>
       <c r="H183" s="22"/>
     </row>
@@ -3862,11 +3857,11 @@
     </row>
     <row r="188" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="23"/>
-      <c r="B188" s="47"/>
-      <c r="C188" s="47"/>
-      <c r="D188" s="47"/>
-      <c r="E188" s="47"/>
-      <c r="F188" s="47"/>
+      <c r="B188" s="55"/>
+      <c r="C188" s="55"/>
+      <c r="D188" s="55"/>
+      <c r="E188" s="55"/>
+      <c r="F188" s="55"/>
       <c r="G188" s="22"/>
       <c r="H188" s="22"/>
     </row>
@@ -3882,21 +3877,21 @@
     </row>
     <row r="190" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="23"/>
-      <c r="B190" s="47"/>
-      <c r="C190" s="47"/>
-      <c r="D190" s="47"/>
-      <c r="E190" s="47"/>
-      <c r="F190" s="47"/>
+      <c r="B190" s="55"/>
+      <c r="C190" s="55"/>
+      <c r="D190" s="55"/>
+      <c r="E190" s="55"/>
+      <c r="F190" s="55"/>
       <c r="G190" s="22"/>
       <c r="H190" s="22"/>
     </row>
     <row r="191" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="18"/>
-      <c r="B191" s="47"/>
-      <c r="C191" s="47"/>
-      <c r="D191" s="47"/>
-      <c r="E191" s="47"/>
-      <c r="F191" s="47"/>
+      <c r="B191" s="55"/>
+      <c r="C191" s="55"/>
+      <c r="D191" s="55"/>
+      <c r="E191" s="55"/>
+      <c r="F191" s="55"/>
       <c r="G191" s="22"/>
       <c r="H191" s="22"/>
     </row>
@@ -3912,61 +3907,61 @@
     </row>
     <row r="193" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="18"/>
-      <c r="B193" s="47"/>
-      <c r="C193" s="47"/>
-      <c r="D193" s="47"/>
-      <c r="E193" s="47"/>
-      <c r="F193" s="47"/>
+      <c r="B193" s="55"/>
+      <c r="C193" s="55"/>
+      <c r="D193" s="55"/>
+      <c r="E193" s="55"/>
+      <c r="F193" s="55"/>
       <c r="G193" s="22"/>
       <c r="H193" s="22"/>
     </row>
     <row r="194" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="18"/>
-      <c r="B194" s="47"/>
-      <c r="C194" s="47"/>
-      <c r="D194" s="47"/>
-      <c r="E194" s="47"/>
-      <c r="F194" s="47"/>
+      <c r="B194" s="55"/>
+      <c r="C194" s="55"/>
+      <c r="D194" s="55"/>
+      <c r="E194" s="55"/>
+      <c r="F194" s="55"/>
       <c r="G194" s="22"/>
       <c r="H194" s="22"/>
     </row>
     <row r="195" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="18"/>
-      <c r="B195" s="47"/>
-      <c r="C195" s="47"/>
-      <c r="D195" s="47"/>
-      <c r="E195" s="47"/>
-      <c r="F195" s="47"/>
+      <c r="B195" s="55"/>
+      <c r="C195" s="55"/>
+      <c r="D195" s="55"/>
+      <c r="E195" s="55"/>
+      <c r="F195" s="55"/>
       <c r="G195" s="22"/>
       <c r="H195" s="22"/>
     </row>
     <row r="196" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="18"/>
-      <c r="B196" s="47"/>
-      <c r="C196" s="47"/>
-      <c r="D196" s="47"/>
-      <c r="E196" s="47"/>
-      <c r="F196" s="47"/>
+      <c r="B196" s="55"/>
+      <c r="C196" s="55"/>
+      <c r="D196" s="55"/>
+      <c r="E196" s="55"/>
+      <c r="F196" s="55"/>
       <c r="G196" s="22"/>
       <c r="H196" s="22"/>
     </row>
     <row r="197" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="18"/>
-      <c r="B197" s="47"/>
-      <c r="C197" s="47"/>
-      <c r="D197" s="47"/>
-      <c r="E197" s="47"/>
-      <c r="F197" s="47"/>
+      <c r="B197" s="55"/>
+      <c r="C197" s="55"/>
+      <c r="D197" s="55"/>
+      <c r="E197" s="55"/>
+      <c r="F197" s="55"/>
       <c r="G197" s="22"/>
       <c r="H197" s="22"/>
     </row>
     <row r="198" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="18"/>
-      <c r="B198" s="47"/>
-      <c r="C198" s="47"/>
-      <c r="D198" s="47"/>
-      <c r="E198" s="47"/>
-      <c r="F198" s="47"/>
+      <c r="B198" s="55"/>
+      <c r="C198" s="55"/>
+      <c r="D198" s="55"/>
+      <c r="E198" s="55"/>
+      <c r="F198" s="55"/>
       <c r="G198" s="22"/>
       <c r="H198" s="22"/>
     </row>
@@ -3982,11 +3977,11 @@
     </row>
     <row r="200" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="23"/>
-      <c r="B200" s="48"/>
-      <c r="C200" s="48"/>
-      <c r="D200" s="48"/>
-      <c r="E200" s="48"/>
-      <c r="F200" s="48"/>
+      <c r="B200" s="56"/>
+      <c r="C200" s="56"/>
+      <c r="D200" s="56"/>
+      <c r="E200" s="56"/>
+      <c r="F200" s="56"/>
       <c r="G200" s="22"/>
       <c r="H200" s="22"/>
     </row>
@@ -4032,11 +4027,11 @@
     </row>
     <row r="205" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="23"/>
-      <c r="B205" s="47"/>
-      <c r="C205" s="47"/>
-      <c r="D205" s="47"/>
-      <c r="E205" s="47"/>
-      <c r="F205" s="47"/>
+      <c r="B205" s="55"/>
+      <c r="C205" s="55"/>
+      <c r="D205" s="55"/>
+      <c r="E205" s="55"/>
+      <c r="F205" s="55"/>
       <c r="G205" s="22"/>
       <c r="H205" s="22"/>
     </row>
@@ -4052,21 +4047,21 @@
     </row>
     <row r="207" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="23"/>
-      <c r="B207" s="47"/>
-      <c r="C207" s="47"/>
-      <c r="D207" s="47"/>
-      <c r="E207" s="47"/>
-      <c r="F207" s="47"/>
+      <c r="B207" s="55"/>
+      <c r="C207" s="55"/>
+      <c r="D207" s="55"/>
+      <c r="E207" s="55"/>
+      <c r="F207" s="55"/>
       <c r="G207" s="22"/>
       <c r="H207" s="22"/>
     </row>
     <row r="208" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="18"/>
-      <c r="B208" s="47"/>
-      <c r="C208" s="47"/>
-      <c r="D208" s="47"/>
-      <c r="E208" s="47"/>
-      <c r="F208" s="47"/>
+      <c r="B208" s="55"/>
+      <c r="C208" s="55"/>
+      <c r="D208" s="55"/>
+      <c r="E208" s="55"/>
+      <c r="F208" s="55"/>
       <c r="G208" s="22"/>
       <c r="H208" s="22"/>
     </row>
@@ -4082,31 +4077,31 @@
     </row>
     <row r="210" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="18"/>
-      <c r="B210" s="47"/>
-      <c r="C210" s="47"/>
-      <c r="D210" s="47"/>
-      <c r="E210" s="47"/>
-      <c r="F210" s="47"/>
+      <c r="B210" s="55"/>
+      <c r="C210" s="55"/>
+      <c r="D210" s="55"/>
+      <c r="E210" s="55"/>
+      <c r="F210" s="55"/>
       <c r="G210" s="22"/>
       <c r="H210" s="22"/>
     </row>
     <row r="211" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="18"/>
-      <c r="B211" s="47"/>
-      <c r="C211" s="47"/>
-      <c r="D211" s="47"/>
-      <c r="E211" s="47"/>
-      <c r="F211" s="47"/>
+      <c r="B211" s="55"/>
+      <c r="C211" s="55"/>
+      <c r="D211" s="55"/>
+      <c r="E211" s="55"/>
+      <c r="F211" s="55"/>
       <c r="G211" s="22"/>
       <c r="H211" s="22"/>
     </row>
     <row r="212" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="18"/>
-      <c r="B212" s="47"/>
-      <c r="C212" s="47"/>
-      <c r="D212" s="47"/>
-      <c r="E212" s="47"/>
-      <c r="F212" s="47"/>
+      <c r="B212" s="55"/>
+      <c r="C212" s="55"/>
+      <c r="D212" s="55"/>
+      <c r="E212" s="55"/>
+      <c r="F212" s="55"/>
       <c r="G212" s="22"/>
       <c r="H212" s="22"/>
     </row>
@@ -4122,11 +4117,11 @@
     </row>
     <row r="214" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="23"/>
-      <c r="B214" s="48"/>
-      <c r="C214" s="48"/>
-      <c r="D214" s="48"/>
-      <c r="E214" s="48"/>
-      <c r="F214" s="48"/>
+      <c r="B214" s="56"/>
+      <c r="C214" s="56"/>
+      <c r="D214" s="56"/>
+      <c r="E214" s="56"/>
+      <c r="F214" s="56"/>
       <c r="G214" s="22"/>
       <c r="H214" s="22"/>
     </row>
@@ -4172,11 +4167,11 @@
     </row>
     <row r="219" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="23"/>
-      <c r="B219" s="47"/>
-      <c r="C219" s="47"/>
-      <c r="D219" s="47"/>
-      <c r="E219" s="47"/>
-      <c r="F219" s="47"/>
+      <c r="B219" s="55"/>
+      <c r="C219" s="55"/>
+      <c r="D219" s="55"/>
+      <c r="E219" s="55"/>
+      <c r="F219" s="55"/>
       <c r="G219" s="22"/>
       <c r="H219" s="22"/>
     </row>
@@ -4192,21 +4187,21 @@
     </row>
     <row r="221" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="23"/>
-      <c r="B221" s="47"/>
-      <c r="C221" s="47"/>
-      <c r="D221" s="47"/>
-      <c r="E221" s="47"/>
-      <c r="F221" s="47"/>
+      <c r="B221" s="55"/>
+      <c r="C221" s="55"/>
+      <c r="D221" s="55"/>
+      <c r="E221" s="55"/>
+      <c r="F221" s="55"/>
       <c r="G221" s="22"/>
       <c r="H221" s="22"/>
     </row>
     <row r="222" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="18"/>
-      <c r="B222" s="47"/>
-      <c r="C222" s="47"/>
-      <c r="D222" s="47"/>
-      <c r="E222" s="47"/>
-      <c r="F222" s="47"/>
+      <c r="B222" s="55"/>
+      <c r="C222" s="55"/>
+      <c r="D222" s="55"/>
+      <c r="E222" s="55"/>
+      <c r="F222" s="55"/>
       <c r="G222" s="22"/>
       <c r="H222" s="22"/>
     </row>
@@ -4222,31 +4217,31 @@
     </row>
     <row r="224" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="18"/>
-      <c r="B224" s="47"/>
-      <c r="C224" s="47"/>
-      <c r="D224" s="47"/>
-      <c r="E224" s="47"/>
-      <c r="F224" s="47"/>
+      <c r="B224" s="55"/>
+      <c r="C224" s="55"/>
+      <c r="D224" s="55"/>
+      <c r="E224" s="55"/>
+      <c r="F224" s="55"/>
       <c r="G224" s="22"/>
       <c r="H224" s="22"/>
     </row>
     <row r="225" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="18"/>
-      <c r="B225" s="47"/>
-      <c r="C225" s="47"/>
-      <c r="D225" s="47"/>
-      <c r="E225" s="47"/>
-      <c r="F225" s="47"/>
+      <c r="B225" s="55"/>
+      <c r="C225" s="55"/>
+      <c r="D225" s="55"/>
+      <c r="E225" s="55"/>
+      <c r="F225" s="55"/>
       <c r="G225" s="22"/>
       <c r="H225" s="22"/>
     </row>
     <row r="226" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="18"/>
-      <c r="B226" s="47"/>
-      <c r="C226" s="47"/>
-      <c r="D226" s="47"/>
-      <c r="E226" s="47"/>
-      <c r="F226" s="47"/>
+      <c r="B226" s="55"/>
+      <c r="C226" s="55"/>
+      <c r="D226" s="55"/>
+      <c r="E226" s="55"/>
+      <c r="F226" s="55"/>
       <c r="G226" s="22"/>
       <c r="H226" s="22"/>
     </row>
@@ -4262,11 +4257,11 @@
     </row>
     <row r="228" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="23"/>
-      <c r="B228" s="48"/>
-      <c r="C228" s="48"/>
-      <c r="D228" s="48"/>
-      <c r="E228" s="48"/>
-      <c r="F228" s="48"/>
+      <c r="B228" s="56"/>
+      <c r="C228" s="56"/>
+      <c r="D228" s="56"/>
+      <c r="E228" s="56"/>
+      <c r="F228" s="56"/>
       <c r="G228" s="22"/>
       <c r="H228" s="22"/>
     </row>
@@ -4304,9 +4299,9 @@
       <c r="A232" s="18"/>
       <c r="B232" s="21"/>
       <c r="C232" s="21"/>
-      <c r="D232" s="47"/>
-      <c r="E232" s="47"/>
-      <c r="F232" s="47"/>
+      <c r="D232" s="55"/>
+      <c r="E232" s="55"/>
+      <c r="F232" s="55"/>
       <c r="G232" s="22"/>
       <c r="H232" s="22"/>
     </row>
@@ -4332,21 +4327,21 @@
     </row>
     <row r="235" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="23"/>
-      <c r="B235" s="47"/>
-      <c r="C235" s="47"/>
-      <c r="D235" s="47"/>
-      <c r="E235" s="47"/>
-      <c r="F235" s="47"/>
+      <c r="B235" s="55"/>
+      <c r="C235" s="55"/>
+      <c r="D235" s="55"/>
+      <c r="E235" s="55"/>
+      <c r="F235" s="55"/>
       <c r="G235" s="22"/>
       <c r="H235" s="22"/>
     </row>
     <row r="236" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="18"/>
-      <c r="B236" s="47"/>
-      <c r="C236" s="47"/>
-      <c r="D236" s="47"/>
-      <c r="E236" s="47"/>
-      <c r="F236" s="47"/>
+      <c r="B236" s="55"/>
+      <c r="C236" s="55"/>
+      <c r="D236" s="55"/>
+      <c r="E236" s="55"/>
+      <c r="F236" s="55"/>
       <c r="G236" s="22"/>
       <c r="H236" s="22"/>
     </row>
@@ -4362,31 +4357,31 @@
     </row>
     <row r="238" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="18"/>
-      <c r="B238" s="47"/>
-      <c r="C238" s="47"/>
-      <c r="D238" s="47"/>
-      <c r="E238" s="47"/>
-      <c r="F238" s="47"/>
+      <c r="B238" s="55"/>
+      <c r="C238" s="55"/>
+      <c r="D238" s="55"/>
+      <c r="E238" s="55"/>
+      <c r="F238" s="55"/>
       <c r="G238" s="22"/>
       <c r="H238" s="22"/>
     </row>
     <row r="239" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="18"/>
-      <c r="B239" s="47"/>
-      <c r="C239" s="47"/>
-      <c r="D239" s="47"/>
-      <c r="E239" s="47"/>
-      <c r="F239" s="47"/>
+      <c r="B239" s="55"/>
+      <c r="C239" s="55"/>
+      <c r="D239" s="55"/>
+      <c r="E239" s="55"/>
+      <c r="F239" s="55"/>
       <c r="G239" s="22"/>
       <c r="H239" s="22"/>
     </row>
     <row r="240" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="18"/>
-      <c r="B240" s="47"/>
-      <c r="C240" s="47"/>
-      <c r="D240" s="47"/>
-      <c r="E240" s="47"/>
-      <c r="F240" s="47"/>
+      <c r="B240" s="55"/>
+      <c r="C240" s="55"/>
+      <c r="D240" s="55"/>
+      <c r="E240" s="55"/>
+      <c r="F240" s="55"/>
       <c r="G240" s="22"/>
       <c r="H240" s="22"/>
     </row>
@@ -4402,11 +4397,11 @@
     </row>
     <row r="242" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="23"/>
-      <c r="B242" s="48"/>
-      <c r="C242" s="48"/>
-      <c r="D242" s="48"/>
-      <c r="E242" s="48"/>
-      <c r="F242" s="48"/>
+      <c r="B242" s="56"/>
+      <c r="C242" s="56"/>
+      <c r="D242" s="56"/>
+      <c r="E242" s="56"/>
+      <c r="F242" s="56"/>
       <c r="G242" s="22"/>
       <c r="H242" s="22"/>
     </row>
@@ -4444,19 +4439,19 @@
       <c r="A246" s="18"/>
       <c r="B246" s="21"/>
       <c r="C246" s="21"/>
-      <c r="D246" s="47"/>
-      <c r="E246" s="47"/>
-      <c r="F246" s="47"/>
+      <c r="D246" s="55"/>
+      <c r="E246" s="55"/>
+      <c r="F246" s="55"/>
       <c r="G246" s="22"/>
       <c r="H246" s="22"/>
     </row>
     <row r="247" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="23"/>
-      <c r="B247" s="47"/>
-      <c r="C247" s="47"/>
-      <c r="D247" s="47"/>
-      <c r="E247" s="47"/>
-      <c r="F247" s="47"/>
+      <c r="B247" s="55"/>
+      <c r="C247" s="55"/>
+      <c r="D247" s="55"/>
+      <c r="E247" s="55"/>
+      <c r="F247" s="55"/>
       <c r="G247" s="22"/>
       <c r="H247" s="22"/>
     </row>
@@ -4472,21 +4467,21 @@
     </row>
     <row r="249" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="23"/>
-      <c r="B249" s="47"/>
-      <c r="C249" s="47"/>
-      <c r="D249" s="47"/>
-      <c r="E249" s="47"/>
-      <c r="F249" s="47"/>
+      <c r="B249" s="55"/>
+      <c r="C249" s="55"/>
+      <c r="D249" s="55"/>
+      <c r="E249" s="55"/>
+      <c r="F249" s="55"/>
       <c r="G249" s="22"/>
       <c r="H249" s="22"/>
     </row>
     <row r="250" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="18"/>
-      <c r="B250" s="47"/>
-      <c r="C250" s="47"/>
-      <c r="D250" s="47"/>
-      <c r="E250" s="47"/>
-      <c r="F250" s="47"/>
+      <c r="B250" s="55"/>
+      <c r="C250" s="55"/>
+      <c r="D250" s="55"/>
+      <c r="E250" s="55"/>
+      <c r="F250" s="55"/>
       <c r="G250" s="22"/>
       <c r="H250" s="22"/>
     </row>
@@ -4502,31 +4497,31 @@
     </row>
     <row r="252" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="18"/>
-      <c r="B252" s="47"/>
-      <c r="C252" s="47"/>
-      <c r="D252" s="47"/>
-      <c r="E252" s="47"/>
-      <c r="F252" s="47"/>
+      <c r="B252" s="55"/>
+      <c r="C252" s="55"/>
+      <c r="D252" s="55"/>
+      <c r="E252" s="55"/>
+      <c r="F252" s="55"/>
       <c r="G252" s="22"/>
       <c r="H252" s="22"/>
     </row>
     <row r="253" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="18"/>
-      <c r="B253" s="47"/>
-      <c r="C253" s="47"/>
-      <c r="D253" s="47"/>
-      <c r="E253" s="47"/>
-      <c r="F253" s="47"/>
+      <c r="B253" s="55"/>
+      <c r="C253" s="55"/>
+      <c r="D253" s="55"/>
+      <c r="E253" s="55"/>
+      <c r="F253" s="55"/>
       <c r="G253" s="22"/>
       <c r="H253" s="22"/>
     </row>
     <row r="254" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="18"/>
-      <c r="B254" s="47"/>
-      <c r="C254" s="47"/>
-      <c r="D254" s="47"/>
-      <c r="E254" s="47"/>
-      <c r="F254" s="47"/>
+      <c r="B254" s="55"/>
+      <c r="C254" s="55"/>
+      <c r="D254" s="55"/>
+      <c r="E254" s="55"/>
+      <c r="F254" s="55"/>
       <c r="G254" s="22"/>
       <c r="H254" s="22"/>
     </row>
@@ -4542,11 +4537,11 @@
     </row>
     <row r="256" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="23"/>
-      <c r="B256" s="48"/>
-      <c r="C256" s="48"/>
-      <c r="D256" s="48"/>
-      <c r="E256" s="48"/>
-      <c r="F256" s="48"/>
+      <c r="B256" s="56"/>
+      <c r="C256" s="56"/>
+      <c r="D256" s="56"/>
+      <c r="E256" s="56"/>
+      <c r="F256" s="56"/>
       <c r="G256" s="22"/>
       <c r="H256" s="22"/>
     </row>
@@ -4592,41 +4587,41 @@
     </row>
     <row r="261" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="23"/>
-      <c r="B261" s="54"/>
-      <c r="C261" s="54"/>
-      <c r="D261" s="54"/>
-      <c r="E261" s="54"/>
-      <c r="F261" s="54"/>
+      <c r="B261" s="57"/>
+      <c r="C261" s="57"/>
+      <c r="D261" s="57"/>
+      <c r="E261" s="57"/>
+      <c r="F261" s="57"/>
       <c r="G261" s="22"/>
       <c r="H261" s="22"/>
     </row>
     <row r="262" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="23"/>
-      <c r="B262" s="47"/>
-      <c r="C262" s="47"/>
-      <c r="D262" s="47"/>
-      <c r="E262" s="47"/>
-      <c r="F262" s="47"/>
+      <c r="B262" s="55"/>
+      <c r="C262" s="55"/>
+      <c r="D262" s="55"/>
+      <c r="E262" s="55"/>
+      <c r="F262" s="55"/>
       <c r="G262" s="22"/>
       <c r="H262" s="22"/>
     </row>
     <row r="263" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="23"/>
-      <c r="B263" s="47"/>
-      <c r="C263" s="47"/>
-      <c r="D263" s="47"/>
-      <c r="E263" s="47"/>
-      <c r="F263" s="47"/>
+      <c r="B263" s="55"/>
+      <c r="C263" s="55"/>
+      <c r="D263" s="55"/>
+      <c r="E263" s="55"/>
+      <c r="F263" s="55"/>
       <c r="G263" s="22"/>
       <c r="H263" s="22"/>
     </row>
     <row r="264" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="18"/>
-      <c r="B264" s="47"/>
-      <c r="C264" s="47"/>
-      <c r="D264" s="47"/>
-      <c r="E264" s="47"/>
-      <c r="F264" s="47"/>
+      <c r="B264" s="55"/>
+      <c r="C264" s="55"/>
+      <c r="D264" s="55"/>
+      <c r="E264" s="55"/>
+      <c r="F264" s="55"/>
       <c r="G264" s="22"/>
       <c r="H264" s="22"/>
     </row>
@@ -4642,31 +4637,31 @@
     </row>
     <row r="266" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A266" s="18"/>
-      <c r="B266" s="47"/>
-      <c r="C266" s="47"/>
-      <c r="D266" s="47"/>
-      <c r="E266" s="47"/>
-      <c r="F266" s="47"/>
+      <c r="B266" s="55"/>
+      <c r="C266" s="55"/>
+      <c r="D266" s="55"/>
+      <c r="E266" s="55"/>
+      <c r="F266" s="55"/>
       <c r="G266" s="22"/>
       <c r="H266" s="22"/>
     </row>
     <row r="267" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267" s="18"/>
-      <c r="B267" s="47"/>
-      <c r="C267" s="47"/>
-      <c r="D267" s="47"/>
-      <c r="E267" s="47"/>
-      <c r="F267" s="47"/>
+      <c r="B267" s="55"/>
+      <c r="C267" s="55"/>
+      <c r="D267" s="55"/>
+      <c r="E267" s="55"/>
+      <c r="F267" s="55"/>
       <c r="G267" s="22"/>
       <c r="H267" s="22"/>
     </row>
     <row r="268" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" s="21"/>
-      <c r="B268" s="47"/>
-      <c r="C268" s="47"/>
-      <c r="D268" s="47"/>
-      <c r="E268" s="47"/>
-      <c r="F268" s="47"/>
+      <c r="B268" s="55"/>
+      <c r="C268" s="55"/>
+      <c r="D268" s="55"/>
+      <c r="E268" s="55"/>
+      <c r="F268" s="55"/>
       <c r="G268" s="22"/>
       <c r="H268" s="22"/>
     </row>
@@ -4682,11 +4677,11 @@
     </row>
     <row r="270" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="23"/>
-      <c r="B270" s="48"/>
-      <c r="C270" s="48"/>
-      <c r="D270" s="48"/>
-      <c r="E270" s="48"/>
-      <c r="F270" s="48"/>
+      <c r="B270" s="56"/>
+      <c r="C270" s="56"/>
+      <c r="D270" s="56"/>
+      <c r="E270" s="56"/>
+      <c r="F270" s="56"/>
       <c r="G270" s="22"/>
       <c r="H270" s="22"/>
     </row>
@@ -4742,31 +4737,31 @@
     </row>
     <row r="276" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A276" s="23"/>
-      <c r="B276" s="47"/>
-      <c r="C276" s="47"/>
-      <c r="D276" s="47"/>
-      <c r="E276" s="47"/>
-      <c r="F276" s="47"/>
+      <c r="B276" s="55"/>
+      <c r="C276" s="55"/>
+      <c r="D276" s="55"/>
+      <c r="E276" s="55"/>
+      <c r="F276" s="55"/>
       <c r="G276" s="22"/>
       <c r="H276" s="22"/>
     </row>
     <row r="277" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A277" s="23"/>
-      <c r="B277" s="47"/>
-      <c r="C277" s="47"/>
-      <c r="D277" s="47"/>
-      <c r="E277" s="47"/>
-      <c r="F277" s="47"/>
+      <c r="B277" s="55"/>
+      <c r="C277" s="55"/>
+      <c r="D277" s="55"/>
+      <c r="E277" s="55"/>
+      <c r="F277" s="55"/>
       <c r="G277" s="22"/>
       <c r="H277" s="22"/>
     </row>
     <row r="278" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A278" s="18"/>
-      <c r="B278" s="47"/>
-      <c r="C278" s="47"/>
-      <c r="D278" s="47"/>
-      <c r="E278" s="47"/>
-      <c r="F278" s="47"/>
+      <c r="B278" s="55"/>
+      <c r="C278" s="55"/>
+      <c r="D278" s="55"/>
+      <c r="E278" s="55"/>
+      <c r="F278" s="55"/>
       <c r="G278" s="22"/>
       <c r="H278" s="22"/>
     </row>
@@ -4782,31 +4777,31 @@
     </row>
     <row r="280" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A280" s="18"/>
-      <c r="B280" s="47"/>
-      <c r="C280" s="47"/>
-      <c r="D280" s="47"/>
-      <c r="E280" s="47"/>
-      <c r="F280" s="47"/>
+      <c r="B280" s="55"/>
+      <c r="C280" s="55"/>
+      <c r="D280" s="55"/>
+      <c r="E280" s="55"/>
+      <c r="F280" s="55"/>
       <c r="G280" s="22"/>
       <c r="H280" s="22"/>
     </row>
     <row r="281" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A281" s="18"/>
-      <c r="B281" s="47"/>
-      <c r="C281" s="47"/>
-      <c r="D281" s="47"/>
-      <c r="E281" s="47"/>
-      <c r="F281" s="47"/>
+      <c r="B281" s="55"/>
+      <c r="C281" s="55"/>
+      <c r="D281" s="55"/>
+      <c r="E281" s="55"/>
+      <c r="F281" s="55"/>
       <c r="G281" s="22"/>
       <c r="H281" s="22"/>
     </row>
     <row r="282" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A282" s="21"/>
-      <c r="B282" s="47"/>
-      <c r="C282" s="47"/>
-      <c r="D282" s="47"/>
-      <c r="E282" s="47"/>
-      <c r="F282" s="47"/>
+      <c r="B282" s="55"/>
+      <c r="C282" s="55"/>
+      <c r="D282" s="55"/>
+      <c r="E282" s="55"/>
+      <c r="F282" s="55"/>
       <c r="G282" s="22"/>
       <c r="H282" s="22"/>
     </row>
@@ -4822,11 +4817,11 @@
     </row>
     <row r="284" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A284" s="23"/>
-      <c r="B284" s="48"/>
-      <c r="C284" s="48"/>
-      <c r="D284" s="48"/>
-      <c r="E284" s="48"/>
-      <c r="F284" s="48"/>
+      <c r="B284" s="56"/>
+      <c r="C284" s="56"/>
+      <c r="D284" s="56"/>
+      <c r="E284" s="56"/>
+      <c r="F284" s="56"/>
       <c r="G284" s="22"/>
       <c r="H284" s="22"/>
     </row>
@@ -4883,30 +4878,30 @@
     <row r="290" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A290" s="23"/>
       <c r="B290" s="21"/>
-      <c r="C290" s="47"/>
-      <c r="D290" s="47"/>
-      <c r="E290" s="47"/>
-      <c r="F290" s="47"/>
+      <c r="C290" s="55"/>
+      <c r="D290" s="55"/>
+      <c r="E290" s="55"/>
+      <c r="F290" s="55"/>
       <c r="G290" s="22"/>
       <c r="H290" s="22"/>
     </row>
     <row r="291" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A291" s="23"/>
       <c r="B291" s="21"/>
-      <c r="C291" s="47"/>
-      <c r="D291" s="47"/>
-      <c r="E291" s="47"/>
-      <c r="F291" s="47"/>
+      <c r="C291" s="55"/>
+      <c r="D291" s="55"/>
+      <c r="E291" s="55"/>
+      <c r="F291" s="55"/>
       <c r="G291" s="22"/>
       <c r="H291" s="22"/>
     </row>
     <row r="292" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A292" s="18"/>
       <c r="B292" s="21"/>
-      <c r="C292" s="47"/>
-      <c r="D292" s="47"/>
-      <c r="E292" s="47"/>
-      <c r="F292" s="47"/>
+      <c r="C292" s="55"/>
+      <c r="D292" s="55"/>
+      <c r="E292" s="55"/>
+      <c r="F292" s="55"/>
       <c r="G292" s="22"/>
       <c r="H292" s="22"/>
     </row>
@@ -4923,30 +4918,30 @@
     <row r="294" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A294" s="18"/>
       <c r="B294" s="21"/>
-      <c r="C294" s="47"/>
-      <c r="D294" s="47"/>
-      <c r="E294" s="47"/>
-      <c r="F294" s="47"/>
+      <c r="C294" s="55"/>
+      <c r="D294" s="55"/>
+      <c r="E294" s="55"/>
+      <c r="F294" s="55"/>
       <c r="G294" s="22"/>
       <c r="H294" s="22"/>
     </row>
     <row r="295" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A295" s="18"/>
       <c r="B295" s="21"/>
-      <c r="C295" s="47"/>
-      <c r="D295" s="47"/>
-      <c r="E295" s="47"/>
-      <c r="F295" s="47"/>
+      <c r="C295" s="55"/>
+      <c r="D295" s="55"/>
+      <c r="E295" s="55"/>
+      <c r="F295" s="55"/>
       <c r="G295" s="22"/>
       <c r="H295" s="22"/>
     </row>
     <row r="296" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A296" s="21"/>
       <c r="B296" s="21"/>
-      <c r="C296" s="47"/>
-      <c r="D296" s="47"/>
-      <c r="E296" s="47"/>
-      <c r="F296" s="47"/>
+      <c r="C296" s="55"/>
+      <c r="D296" s="55"/>
+      <c r="E296" s="55"/>
+      <c r="F296" s="55"/>
       <c r="G296" s="22"/>
       <c r="H296" s="22"/>
     </row>
@@ -4963,10 +4958,10 @@
     <row r="298" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A298" s="23"/>
       <c r="B298" s="1"/>
-      <c r="C298" s="48"/>
-      <c r="D298" s="48"/>
-      <c r="E298" s="48"/>
-      <c r="F298" s="48"/>
+      <c r="C298" s="56"/>
+      <c r="D298" s="56"/>
+      <c r="E298" s="56"/>
+      <c r="F298" s="56"/>
       <c r="G298" s="22"/>
       <c r="H298" s="22"/>
     </row>
@@ -5022,31 +5017,31 @@
     </row>
     <row r="304" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="23"/>
-      <c r="B304" s="47"/>
-      <c r="C304" s="47"/>
-      <c r="D304" s="47"/>
-      <c r="E304" s="47"/>
-      <c r="F304" s="47"/>
+      <c r="B304" s="55"/>
+      <c r="C304" s="55"/>
+      <c r="D304" s="55"/>
+      <c r="E304" s="55"/>
+      <c r="F304" s="55"/>
       <c r="G304" s="22"/>
       <c r="H304" s="22"/>
     </row>
     <row r="305" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A305" s="23"/>
-      <c r="B305" s="47"/>
-      <c r="C305" s="47"/>
-      <c r="D305" s="47"/>
-      <c r="E305" s="47"/>
-      <c r="F305" s="47"/>
+      <c r="B305" s="55"/>
+      <c r="C305" s="55"/>
+      <c r="D305" s="55"/>
+      <c r="E305" s="55"/>
+      <c r="F305" s="55"/>
       <c r="G305" s="22"/>
       <c r="H305" s="22"/>
     </row>
     <row r="306" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A306" s="18"/>
-      <c r="B306" s="47"/>
-      <c r="C306" s="47"/>
-      <c r="D306" s="47"/>
-      <c r="E306" s="47"/>
-      <c r="F306" s="47"/>
+      <c r="B306" s="55"/>
+      <c r="C306" s="55"/>
+      <c r="D306" s="55"/>
+      <c r="E306" s="55"/>
+      <c r="F306" s="55"/>
       <c r="G306" s="22"/>
       <c r="H306" s="22"/>
     </row>
@@ -5062,31 +5057,31 @@
     </row>
     <row r="308" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A308" s="18"/>
-      <c r="B308" s="47"/>
-      <c r="C308" s="47"/>
-      <c r="D308" s="47"/>
-      <c r="E308" s="47"/>
-      <c r="F308" s="47"/>
+      <c r="B308" s="55"/>
+      <c r="C308" s="55"/>
+      <c r="D308" s="55"/>
+      <c r="E308" s="55"/>
+      <c r="F308" s="55"/>
       <c r="G308" s="22"/>
       <c r="H308" s="22"/>
     </row>
     <row r="309" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A309" s="18"/>
-      <c r="B309" s="47"/>
-      <c r="C309" s="47"/>
-      <c r="D309" s="47"/>
-      <c r="E309" s="47"/>
-      <c r="F309" s="47"/>
+      <c r="B309" s="55"/>
+      <c r="C309" s="55"/>
+      <c r="D309" s="55"/>
+      <c r="E309" s="55"/>
+      <c r="F309" s="55"/>
       <c r="G309" s="22"/>
       <c r="H309" s="22"/>
     </row>
     <row r="310" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A310" s="21"/>
-      <c r="B310" s="47"/>
-      <c r="C310" s="47"/>
-      <c r="D310" s="47"/>
-      <c r="E310" s="47"/>
-      <c r="F310" s="47"/>
+      <c r="B310" s="55"/>
+      <c r="C310" s="55"/>
+      <c r="D310" s="55"/>
+      <c r="E310" s="55"/>
+      <c r="F310" s="55"/>
       <c r="G310" s="22"/>
       <c r="H310" s="22"/>
     </row>
@@ -5102,11 +5097,11 @@
     </row>
     <row r="312" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A312" s="23"/>
-      <c r="B312" s="48"/>
-      <c r="C312" s="48"/>
-      <c r="D312" s="48"/>
-      <c r="E312" s="48"/>
-      <c r="F312" s="48"/>
+      <c r="B312" s="56"/>
+      <c r="C312" s="56"/>
+      <c r="D312" s="56"/>
+      <c r="E312" s="56"/>
+      <c r="F312" s="56"/>
       <c r="G312" s="22"/>
       <c r="H312" s="22"/>
     </row>
@@ -5162,31 +5157,31 @@
     </row>
     <row r="318" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A318" s="23"/>
-      <c r="B318" s="47"/>
-      <c r="C318" s="47"/>
-      <c r="D318" s="47"/>
-      <c r="E318" s="47"/>
-      <c r="F318" s="47"/>
+      <c r="B318" s="55"/>
+      <c r="C318" s="55"/>
+      <c r="D318" s="55"/>
+      <c r="E318" s="55"/>
+      <c r="F318" s="55"/>
       <c r="G318" s="22"/>
       <c r="H318" s="22"/>
     </row>
     <row r="319" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A319" s="23"/>
-      <c r="B319" s="47"/>
-      <c r="C319" s="47"/>
-      <c r="D319" s="47"/>
-      <c r="E319" s="47"/>
-      <c r="F319" s="47"/>
+      <c r="B319" s="55"/>
+      <c r="C319" s="55"/>
+      <c r="D319" s="55"/>
+      <c r="E319" s="55"/>
+      <c r="F319" s="55"/>
       <c r="G319" s="22"/>
       <c r="H319" s="22"/>
     </row>
     <row r="320" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A320" s="18"/>
-      <c r="B320" s="47"/>
-      <c r="C320" s="47"/>
-      <c r="D320" s="47"/>
-      <c r="E320" s="47"/>
-      <c r="F320" s="47"/>
+      <c r="B320" s="55"/>
+      <c r="C320" s="55"/>
+      <c r="D320" s="55"/>
+      <c r="E320" s="55"/>
+      <c r="F320" s="55"/>
       <c r="G320" s="22"/>
       <c r="H320" s="22"/>
     </row>
@@ -5202,31 +5197,31 @@
     </row>
     <row r="322" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A322" s="18"/>
-      <c r="B322" s="47"/>
-      <c r="C322" s="47"/>
-      <c r="D322" s="47"/>
-      <c r="E322" s="47"/>
-      <c r="F322" s="47"/>
+      <c r="B322" s="55"/>
+      <c r="C322" s="55"/>
+      <c r="D322" s="55"/>
+      <c r="E322" s="55"/>
+      <c r="F322" s="55"/>
       <c r="G322" s="22"/>
       <c r="H322" s="22"/>
     </row>
     <row r="323" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A323" s="18"/>
-      <c r="B323" s="47"/>
-      <c r="C323" s="47"/>
-      <c r="D323" s="47"/>
-      <c r="E323" s="47"/>
-      <c r="F323" s="47"/>
+      <c r="B323" s="55"/>
+      <c r="C323" s="55"/>
+      <c r="D323" s="55"/>
+      <c r="E323" s="55"/>
+      <c r="F323" s="55"/>
       <c r="G323" s="22"/>
       <c r="H323" s="22"/>
     </row>
     <row r="324" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A324" s="21"/>
-      <c r="B324" s="47"/>
-      <c r="C324" s="47"/>
-      <c r="D324" s="47"/>
-      <c r="E324" s="47"/>
-      <c r="F324" s="47"/>
+      <c r="B324" s="55"/>
+      <c r="C324" s="55"/>
+      <c r="D324" s="55"/>
+      <c r="E324" s="55"/>
+      <c r="F324" s="55"/>
       <c r="G324" s="22"/>
       <c r="H324" s="22"/>
     </row>
@@ -5242,11 +5237,11 @@
     </row>
     <row r="326" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A326" s="23"/>
-      <c r="B326" s="48"/>
-      <c r="C326" s="48"/>
-      <c r="D326" s="48"/>
-      <c r="E326" s="48"/>
-      <c r="F326" s="48"/>
+      <c r="B326" s="56"/>
+      <c r="C326" s="56"/>
+      <c r="D326" s="56"/>
+      <c r="E326" s="56"/>
+      <c r="F326" s="56"/>
       <c r="G326" s="22"/>
       <c r="H326" s="22"/>
     </row>
@@ -5292,41 +5287,41 @@
     </row>
     <row r="331" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A331" s="23"/>
-      <c r="B331" s="47"/>
-      <c r="C331" s="47"/>
-      <c r="D331" s="47"/>
-      <c r="E331" s="47"/>
-      <c r="F331" s="47"/>
+      <c r="B331" s="55"/>
+      <c r="C331" s="55"/>
+      <c r="D331" s="55"/>
+      <c r="E331" s="55"/>
+      <c r="F331" s="55"/>
       <c r="G331" s="22"/>
       <c r="H331" s="22"/>
     </row>
     <row r="332" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A332" s="23"/>
-      <c r="B332" s="47"/>
-      <c r="C332" s="47"/>
-      <c r="D332" s="47"/>
-      <c r="E332" s="47"/>
-      <c r="F332" s="47"/>
+      <c r="B332" s="55"/>
+      <c r="C332" s="55"/>
+      <c r="D332" s="55"/>
+      <c r="E332" s="55"/>
+      <c r="F332" s="55"/>
       <c r="G332" s="22"/>
       <c r="H332" s="22"/>
     </row>
     <row r="333" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A333" s="23"/>
-      <c r="B333" s="47"/>
-      <c r="C333" s="47"/>
-      <c r="D333" s="47"/>
-      <c r="E333" s="47"/>
-      <c r="F333" s="47"/>
+      <c r="B333" s="55"/>
+      <c r="C333" s="55"/>
+      <c r="D333" s="55"/>
+      <c r="E333" s="55"/>
+      <c r="F333" s="55"/>
       <c r="G333" s="22"/>
       <c r="H333" s="22"/>
     </row>
     <row r="334" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A334" s="18"/>
-      <c r="B334" s="47"/>
-      <c r="C334" s="47"/>
-      <c r="D334" s="47"/>
-      <c r="E334" s="47"/>
-      <c r="F334" s="47"/>
+      <c r="B334" s="55"/>
+      <c r="C334" s="55"/>
+      <c r="D334" s="55"/>
+      <c r="E334" s="55"/>
+      <c r="F334" s="55"/>
       <c r="G334" s="22"/>
       <c r="H334" s="22"/>
     </row>
@@ -5352,31 +5347,31 @@
     </row>
     <row r="337" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A337" s="18"/>
-      <c r="B337" s="47"/>
-      <c r="C337" s="47"/>
-      <c r="D337" s="47"/>
-      <c r="E337" s="47"/>
-      <c r="F337" s="47"/>
+      <c r="B337" s="55"/>
+      <c r="C337" s="55"/>
+      <c r="D337" s="55"/>
+      <c r="E337" s="55"/>
+      <c r="F337" s="55"/>
       <c r="G337" s="22"/>
       <c r="H337" s="22"/>
     </row>
     <row r="338" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A338" s="21"/>
-      <c r="B338" s="47"/>
-      <c r="C338" s="47"/>
-      <c r="D338" s="47"/>
-      <c r="E338" s="47"/>
-      <c r="F338" s="47"/>
+      <c r="B338" s="55"/>
+      <c r="C338" s="55"/>
+      <c r="D338" s="55"/>
+      <c r="E338" s="55"/>
+      <c r="F338" s="55"/>
       <c r="G338" s="22"/>
       <c r="H338" s="22"/>
     </row>
     <row r="339" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A339" s="21"/>
-      <c r="B339" s="47"/>
-      <c r="C339" s="47"/>
-      <c r="D339" s="47"/>
-      <c r="E339" s="47"/>
-      <c r="F339" s="47"/>
+      <c r="B339" s="55"/>
+      <c r="C339" s="55"/>
+      <c r="D339" s="55"/>
+      <c r="E339" s="55"/>
+      <c r="F339" s="55"/>
       <c r="G339" s="22"/>
       <c r="H339" s="22"/>
     </row>
@@ -5392,11 +5387,11 @@
     </row>
     <row r="341" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A341" s="23"/>
-      <c r="B341" s="48"/>
-      <c r="C341" s="48"/>
-      <c r="D341" s="48"/>
-      <c r="E341" s="48"/>
-      <c r="F341" s="48"/>
+      <c r="B341" s="56"/>
+      <c r="C341" s="56"/>
+      <c r="D341" s="56"/>
+      <c r="E341" s="56"/>
+      <c r="F341" s="56"/>
       <c r="G341" s="22"/>
       <c r="H341" s="22"/>
     </row>
@@ -5442,41 +5437,41 @@
     </row>
     <row r="346" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A346" s="23"/>
-      <c r="B346" s="47"/>
-      <c r="C346" s="47"/>
-      <c r="D346" s="47"/>
-      <c r="E346" s="47"/>
-      <c r="F346" s="47"/>
+      <c r="B346" s="55"/>
+      <c r="C346" s="55"/>
+      <c r="D346" s="55"/>
+      <c r="E346" s="55"/>
+      <c r="F346" s="55"/>
       <c r="G346" s="22"/>
       <c r="H346" s="22"/>
     </row>
     <row r="347" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A347" s="23"/>
-      <c r="B347" s="47"/>
-      <c r="C347" s="47"/>
-      <c r="D347" s="47"/>
-      <c r="E347" s="47"/>
-      <c r="F347" s="47"/>
+      <c r="B347" s="55"/>
+      <c r="C347" s="55"/>
+      <c r="D347" s="55"/>
+      <c r="E347" s="55"/>
+      <c r="F347" s="55"/>
       <c r="G347" s="22"/>
       <c r="H347" s="22"/>
     </row>
     <row r="348" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A348" s="23"/>
-      <c r="B348" s="47"/>
-      <c r="C348" s="47"/>
-      <c r="D348" s="47"/>
-      <c r="E348" s="47"/>
-      <c r="F348" s="47"/>
+      <c r="B348" s="55"/>
+      <c r="C348" s="55"/>
+      <c r="D348" s="55"/>
+      <c r="E348" s="55"/>
+      <c r="F348" s="55"/>
       <c r="G348" s="22"/>
       <c r="H348" s="22"/>
     </row>
     <row r="349" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A349" s="18"/>
-      <c r="B349" s="47"/>
-      <c r="C349" s="47"/>
-      <c r="D349" s="47"/>
-      <c r="E349" s="47"/>
-      <c r="F349" s="47"/>
+      <c r="B349" s="55"/>
+      <c r="C349" s="55"/>
+      <c r="D349" s="55"/>
+      <c r="E349" s="55"/>
+      <c r="F349" s="55"/>
       <c r="G349" s="22"/>
       <c r="H349" s="22"/>
     </row>
@@ -5492,41 +5487,41 @@
     </row>
     <row r="351" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A351" s="18"/>
-      <c r="B351" s="47"/>
-      <c r="C351" s="47"/>
-      <c r="D351" s="47"/>
-      <c r="E351" s="47"/>
-      <c r="F351" s="47"/>
+      <c r="B351" s="55"/>
+      <c r="C351" s="55"/>
+      <c r="D351" s="55"/>
+      <c r="E351" s="55"/>
+      <c r="F351" s="55"/>
       <c r="G351" s="22"/>
       <c r="H351" s="22"/>
     </row>
     <row r="352" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A352" s="18"/>
-      <c r="B352" s="47"/>
-      <c r="C352" s="47"/>
-      <c r="D352" s="47"/>
-      <c r="E352" s="47"/>
-      <c r="F352" s="47"/>
+      <c r="B352" s="55"/>
+      <c r="C352" s="55"/>
+      <c r="D352" s="55"/>
+      <c r="E352" s="55"/>
+      <c r="F352" s="55"/>
       <c r="G352" s="22"/>
       <c r="H352" s="22"/>
     </row>
     <row r="353" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A353" s="21"/>
-      <c r="B353" s="47"/>
-      <c r="C353" s="47"/>
-      <c r="D353" s="47"/>
-      <c r="E353" s="47"/>
-      <c r="F353" s="47"/>
+      <c r="B353" s="55"/>
+      <c r="C353" s="55"/>
+      <c r="D353" s="55"/>
+      <c r="E353" s="55"/>
+      <c r="F353" s="55"/>
       <c r="G353" s="22"/>
       <c r="H353" s="22"/>
     </row>
     <row r="354" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A354" s="21"/>
-      <c r="B354" s="47"/>
-      <c r="C354" s="47"/>
-      <c r="D354" s="47"/>
-      <c r="E354" s="47"/>
-      <c r="F354" s="47"/>
+      <c r="B354" s="55"/>
+      <c r="C354" s="55"/>
+      <c r="D354" s="55"/>
+      <c r="E354" s="55"/>
+      <c r="F354" s="55"/>
       <c r="G354" s="22"/>
       <c r="H354" s="22"/>
     </row>
@@ -5542,11 +5537,11 @@
     </row>
     <row r="356" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A356" s="23"/>
-      <c r="B356" s="48"/>
-      <c r="C356" s="48"/>
-      <c r="D356" s="48"/>
-      <c r="E356" s="48"/>
-      <c r="F356" s="48"/>
+      <c r="B356" s="56"/>
+      <c r="C356" s="56"/>
+      <c r="D356" s="56"/>
+      <c r="E356" s="56"/>
+      <c r="F356" s="56"/>
       <c r="G356" s="22"/>
       <c r="H356" s="22"/>
     </row>
@@ -5592,9 +5587,9 @@
     </row>
     <row r="361" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A361" s="23"/>
-      <c r="B361" s="47"/>
-      <c r="C361" s="47"/>
-      <c r="D361" s="47"/>
+      <c r="B361" s="55"/>
+      <c r="C361" s="55"/>
+      <c r="D361" s="55"/>
       <c r="E361" s="21"/>
       <c r="F361" s="24"/>
       <c r="G361" s="22"/>
@@ -5602,9 +5597,9 @@
     </row>
     <row r="362" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A362" s="23"/>
-      <c r="B362" s="47"/>
-      <c r="C362" s="47"/>
-      <c r="D362" s="47"/>
+      <c r="B362" s="55"/>
+      <c r="C362" s="55"/>
+      <c r="D362" s="55"/>
       <c r="E362" s="21"/>
       <c r="F362" s="24"/>
       <c r="G362" s="22"/>
@@ -5612,9 +5607,9 @@
     </row>
     <row r="363" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A363" s="23"/>
-      <c r="B363" s="47"/>
-      <c r="C363" s="47"/>
-      <c r="D363" s="47"/>
+      <c r="B363" s="55"/>
+      <c r="C363" s="55"/>
+      <c r="D363" s="55"/>
       <c r="E363" s="21"/>
       <c r="F363" s="24"/>
       <c r="G363" s="22"/>
@@ -5622,9 +5617,9 @@
     </row>
     <row r="364" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A364" s="18"/>
-      <c r="B364" s="47"/>
-      <c r="C364" s="47"/>
-      <c r="D364" s="47"/>
+      <c r="B364" s="55"/>
+      <c r="C364" s="55"/>
+      <c r="D364" s="55"/>
       <c r="E364" s="21"/>
       <c r="F364" s="24"/>
       <c r="G364" s="22"/>
@@ -5642,9 +5637,9 @@
     </row>
     <row r="366" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A366" s="18"/>
-      <c r="B366" s="47"/>
-      <c r="C366" s="47"/>
-      <c r="D366" s="47"/>
+      <c r="B366" s="55"/>
+      <c r="C366" s="55"/>
+      <c r="D366" s="55"/>
       <c r="E366" s="21"/>
       <c r="F366" s="24"/>
       <c r="G366" s="22"/>
@@ -5652,9 +5647,9 @@
     </row>
     <row r="367" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A367" s="18"/>
-      <c r="B367" s="47"/>
-      <c r="C367" s="47"/>
-      <c r="D367" s="47"/>
+      <c r="B367" s="55"/>
+      <c r="C367" s="55"/>
+      <c r="D367" s="55"/>
       <c r="E367" s="21"/>
       <c r="F367" s="24"/>
       <c r="G367" s="22"/>
@@ -5662,9 +5657,9 @@
     </row>
     <row r="368" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A368" s="21"/>
-      <c r="B368" s="47"/>
-      <c r="C368" s="47"/>
-      <c r="D368" s="47"/>
+      <c r="B368" s="55"/>
+      <c r="C368" s="55"/>
+      <c r="D368" s="55"/>
       <c r="E368" s="21"/>
       <c r="F368" s="24"/>
       <c r="G368" s="22"/>
@@ -5672,9 +5667,9 @@
     </row>
     <row r="369" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A369" s="21"/>
-      <c r="B369" s="47"/>
-      <c r="C369" s="47"/>
-      <c r="D369" s="47"/>
+      <c r="B369" s="55"/>
+      <c r="C369" s="55"/>
+      <c r="D369" s="55"/>
       <c r="E369" s="21"/>
       <c r="F369" s="24"/>
       <c r="G369" s="22"/>
@@ -5692,9 +5687,9 @@
     </row>
     <row r="371" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A371" s="23"/>
-      <c r="B371" s="48"/>
-      <c r="C371" s="48"/>
-      <c r="D371" s="48"/>
+      <c r="B371" s="56"/>
+      <c r="C371" s="56"/>
+      <c r="D371" s="56"/>
       <c r="E371" s="28"/>
       <c r="F371" s="25"/>
       <c r="G371" s="22"/>
@@ -5822,11 +5817,11 @@
     </row>
     <row r="384" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A384" s="23"/>
-      <c r="B384" s="48"/>
-      <c r="C384" s="48"/>
-      <c r="D384" s="48"/>
-      <c r="E384" s="48"/>
-      <c r="F384" s="48"/>
+      <c r="B384" s="56"/>
+      <c r="C384" s="56"/>
+      <c r="D384" s="56"/>
+      <c r="E384" s="56"/>
+      <c r="F384" s="56"/>
       <c r="G384" s="22"/>
       <c r="H384" s="22"/>
     </row>
@@ -5952,11 +5947,11 @@
     </row>
     <row r="397" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A397" s="23"/>
-      <c r="B397" s="48"/>
-      <c r="C397" s="48"/>
-      <c r="D397" s="48"/>
-      <c r="E397" s="48"/>
-      <c r="F397" s="48"/>
+      <c r="B397" s="56"/>
+      <c r="C397" s="56"/>
+      <c r="D397" s="56"/>
+      <c r="E397" s="56"/>
+      <c r="F397" s="56"/>
       <c r="G397" s="22"/>
       <c r="H397" s="22"/>
     </row>
@@ -6082,11 +6077,11 @@
     </row>
     <row r="410" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A410" s="23"/>
-      <c r="B410" s="48"/>
-      <c r="C410" s="48"/>
-      <c r="D410" s="48"/>
-      <c r="E410" s="48"/>
-      <c r="F410" s="48"/>
+      <c r="B410" s="56"/>
+      <c r="C410" s="56"/>
+      <c r="D410" s="56"/>
+      <c r="E410" s="56"/>
+      <c r="F410" s="56"/>
       <c r="G410" s="22"/>
       <c r="H410" s="22"/>
     </row>
@@ -6212,11 +6207,11 @@
     </row>
     <row r="423" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A423" s="23"/>
-      <c r="B423" s="48"/>
-      <c r="C423" s="48"/>
-      <c r="D423" s="48"/>
-      <c r="E423" s="48"/>
-      <c r="F423" s="48"/>
+      <c r="B423" s="56"/>
+      <c r="C423" s="56"/>
+      <c r="D423" s="56"/>
+      <c r="E423" s="56"/>
+      <c r="F423" s="56"/>
       <c r="G423" s="22"/>
       <c r="H423" s="22"/>
     </row>
@@ -6342,11 +6337,11 @@
     </row>
     <row r="436" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A436" s="23"/>
-      <c r="B436" s="48"/>
-      <c r="C436" s="48"/>
-      <c r="D436" s="48"/>
-      <c r="E436" s="48"/>
-      <c r="F436" s="48"/>
+      <c r="B436" s="56"/>
+      <c r="C436" s="56"/>
+      <c r="D436" s="56"/>
+      <c r="E436" s="56"/>
+      <c r="F436" s="56"/>
       <c r="G436" s="22"/>
       <c r="H436" s="22"/>
     </row>
@@ -6472,11 +6467,11 @@
     </row>
     <row r="449" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A449" s="23"/>
-      <c r="B449" s="48"/>
-      <c r="C449" s="48"/>
-      <c r="D449" s="48"/>
-      <c r="E449" s="48"/>
-      <c r="F449" s="48"/>
+      <c r="B449" s="56"/>
+      <c r="C449" s="56"/>
+      <c r="D449" s="56"/>
+      <c r="E449" s="56"/>
+      <c r="F449" s="56"/>
       <c r="G449" s="22"/>
       <c r="H449" s="22"/>
     </row>
@@ -6602,11 +6597,11 @@
     </row>
     <row r="462" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A462" s="23"/>
-      <c r="B462" s="48"/>
-      <c r="C462" s="48"/>
-      <c r="D462" s="48"/>
-      <c r="E462" s="48"/>
-      <c r="F462" s="48"/>
+      <c r="B462" s="56"/>
+      <c r="C462" s="56"/>
+      <c r="D462" s="56"/>
+      <c r="E462" s="56"/>
+      <c r="F462" s="56"/>
       <c r="G462" s="22"/>
       <c r="H462" s="22"/>
     </row>
@@ -6732,11 +6727,11 @@
     </row>
     <row r="475" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A475" s="23"/>
-      <c r="B475" s="48"/>
-      <c r="C475" s="48"/>
-      <c r="D475" s="48"/>
-      <c r="E475" s="48"/>
-      <c r="F475" s="48"/>
+      <c r="B475" s="56"/>
+      <c r="C475" s="56"/>
+      <c r="D475" s="56"/>
+      <c r="E475" s="56"/>
+      <c r="F475" s="56"/>
       <c r="G475" s="22"/>
       <c r="H475" s="22"/>
     </row>
@@ -6863,10 +6858,10 @@
     <row r="488" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A488" s="23"/>
       <c r="B488" s="28"/>
-      <c r="C488" s="48"/>
-      <c r="D488" s="48"/>
-      <c r="E488" s="48"/>
-      <c r="F488" s="48"/>
+      <c r="C488" s="56"/>
+      <c r="D488" s="56"/>
+      <c r="E488" s="56"/>
+      <c r="F488" s="56"/>
       <c r="G488" s="22"/>
       <c r="H488" s="22"/>
     </row>
@@ -6992,11 +6987,11 @@
     </row>
     <row r="501" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A501" s="23"/>
-      <c r="B501" s="48"/>
-      <c r="C501" s="48"/>
-      <c r="D501" s="48"/>
-      <c r="E501" s="48"/>
-      <c r="F501" s="48"/>
+      <c r="B501" s="56"/>
+      <c r="C501" s="56"/>
+      <c r="D501" s="56"/>
+      <c r="E501" s="56"/>
+      <c r="F501" s="56"/>
       <c r="G501" s="22"/>
       <c r="H501" s="22"/>
     </row>
@@ -7122,11 +7117,11 @@
     </row>
     <row r="514" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A514" s="23"/>
-      <c r="B514" s="48"/>
-      <c r="C514" s="48"/>
-      <c r="D514" s="48"/>
-      <c r="E514" s="48"/>
-      <c r="F514" s="48"/>
+      <c r="B514" s="56"/>
+      <c r="C514" s="56"/>
+      <c r="D514" s="56"/>
+      <c r="E514" s="56"/>
+      <c r="F514" s="56"/>
       <c r="G514" s="22"/>
       <c r="H514" s="22"/>
     </row>
@@ -7252,11 +7247,11 @@
     </row>
     <row r="527" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A527" s="23"/>
-      <c r="B527" s="48"/>
-      <c r="C527" s="48"/>
-      <c r="D527" s="48"/>
-      <c r="E527" s="48"/>
-      <c r="F527" s="48"/>
+      <c r="B527" s="56"/>
+      <c r="C527" s="56"/>
+      <c r="D527" s="56"/>
+      <c r="E527" s="56"/>
+      <c r="F527" s="56"/>
       <c r="G527" s="22"/>
       <c r="H527" s="22"/>
     </row>
@@ -7382,11 +7377,11 @@
     </row>
     <row r="540" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A540" s="23"/>
-      <c r="B540" s="48"/>
-      <c r="C540" s="48"/>
-      <c r="D540" s="48"/>
-      <c r="E540" s="48"/>
-      <c r="F540" s="48"/>
+      <c r="B540" s="56"/>
+      <c r="C540" s="56"/>
+      <c r="D540" s="56"/>
+      <c r="E540" s="56"/>
+      <c r="F540" s="56"/>
       <c r="G540" s="22"/>
       <c r="H540" s="22"/>
     </row>
@@ -7512,11 +7507,11 @@
     </row>
     <row r="553" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A553" s="23"/>
-      <c r="B553" s="48"/>
-      <c r="C553" s="48"/>
-      <c r="D553" s="48"/>
-      <c r="E553" s="48"/>
-      <c r="F553" s="48"/>
+      <c r="B553" s="56"/>
+      <c r="C553" s="56"/>
+      <c r="D553" s="56"/>
+      <c r="E553" s="56"/>
+      <c r="F553" s="56"/>
       <c r="G553" s="22"/>
       <c r="H553" s="22"/>
     </row>
@@ -7642,11 +7637,11 @@
     </row>
     <row r="566" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A566" s="23"/>
-      <c r="B566" s="48"/>
-      <c r="C566" s="48"/>
-      <c r="D566" s="48"/>
-      <c r="E566" s="48"/>
-      <c r="F566" s="48"/>
+      <c r="B566" s="56"/>
+      <c r="C566" s="56"/>
+      <c r="D566" s="56"/>
+      <c r="E566" s="56"/>
+      <c r="F566" s="56"/>
       <c r="G566" s="22"/>
       <c r="H566" s="22"/>
     </row>
@@ -7772,11 +7767,11 @@
     </row>
     <row r="579" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A579" s="23"/>
-      <c r="B579" s="48"/>
-      <c r="C579" s="48"/>
-      <c r="D579" s="48"/>
-      <c r="E579" s="48"/>
-      <c r="F579" s="48"/>
+      <c r="B579" s="56"/>
+      <c r="C579" s="56"/>
+      <c r="D579" s="56"/>
+      <c r="E579" s="56"/>
+      <c r="F579" s="56"/>
       <c r="G579" s="22"/>
       <c r="H579" s="22"/>
     </row>
@@ -7902,11 +7897,11 @@
     </row>
     <row r="592" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A592" s="23"/>
-      <c r="B592" s="48"/>
-      <c r="C592" s="48"/>
-      <c r="D592" s="48"/>
-      <c r="E592" s="48"/>
-      <c r="F592" s="48"/>
+      <c r="B592" s="56"/>
+      <c r="C592" s="56"/>
+      <c r="D592" s="56"/>
+      <c r="E592" s="56"/>
+      <c r="F592" s="56"/>
       <c r="G592" s="22"/>
       <c r="H592" s="22"/>
     </row>
@@ -8032,11 +8027,11 @@
     </row>
     <row r="605" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A605" s="23"/>
-      <c r="B605" s="48"/>
-      <c r="C605" s="48"/>
-      <c r="D605" s="48"/>
-      <c r="E605" s="48"/>
-      <c r="F605" s="48"/>
+      <c r="B605" s="56"/>
+      <c r="C605" s="56"/>
+      <c r="D605" s="56"/>
+      <c r="E605" s="56"/>
+      <c r="F605" s="56"/>
       <c r="G605" s="22"/>
       <c r="H605" s="22"/>
     </row>
@@ -8162,11 +8157,11 @@
     </row>
     <row r="618" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A618" s="23"/>
-      <c r="B618" s="48"/>
-      <c r="C618" s="48"/>
-      <c r="D618" s="48"/>
-      <c r="E618" s="48"/>
-      <c r="F618" s="48"/>
+      <c r="B618" s="56"/>
+      <c r="C618" s="56"/>
+      <c r="D618" s="56"/>
+      <c r="E618" s="56"/>
+      <c r="F618" s="56"/>
       <c r="G618" s="22"/>
       <c r="H618" s="22"/>
     </row>
@@ -8292,11 +8287,11 @@
     </row>
     <row r="631" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A631" s="23"/>
-      <c r="B631" s="48"/>
-      <c r="C631" s="48"/>
-      <c r="D631" s="48"/>
-      <c r="E631" s="48"/>
-      <c r="F631" s="48"/>
+      <c r="B631" s="56"/>
+      <c r="C631" s="56"/>
+      <c r="D631" s="56"/>
+      <c r="E631" s="56"/>
+      <c r="F631" s="56"/>
       <c r="G631" s="22"/>
       <c r="H631" s="22"/>
     </row>
@@ -8422,9 +8417,9 @@
     </row>
     <row r="644" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A644" s="23"/>
-      <c r="B644" s="48"/>
-      <c r="C644" s="48"/>
-      <c r="D644" s="48"/>
+      <c r="B644" s="56"/>
+      <c r="C644" s="56"/>
+      <c r="D644" s="56"/>
       <c r="E644" s="28"/>
       <c r="F644" s="28"/>
       <c r="G644" s="22"/>
@@ -8552,11 +8547,11 @@
     </row>
     <row r="657" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A657" s="23"/>
-      <c r="B657" s="48"/>
-      <c r="C657" s="48"/>
-      <c r="D657" s="48"/>
-      <c r="E657" s="48"/>
-      <c r="F657" s="48"/>
+      <c r="B657" s="56"/>
+      <c r="C657" s="56"/>
+      <c r="D657" s="56"/>
+      <c r="E657" s="56"/>
+      <c r="F657" s="56"/>
       <c r="G657" s="22"/>
       <c r="H657" s="22"/>
     </row>
@@ -8682,11 +8677,11 @@
     </row>
     <row r="670" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A670" s="23"/>
-      <c r="B670" s="48"/>
-      <c r="C670" s="48"/>
-      <c r="D670" s="48"/>
-      <c r="E670" s="48"/>
-      <c r="F670" s="48"/>
+      <c r="B670" s="56"/>
+      <c r="C670" s="56"/>
+      <c r="D670" s="56"/>
+      <c r="E670" s="56"/>
+      <c r="F670" s="56"/>
       <c r="G670" s="22"/>
       <c r="H670" s="22"/>
     </row>
@@ -8812,11 +8807,11 @@
     </row>
     <row r="683" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A683" s="23"/>
-      <c r="B683" s="48"/>
-      <c r="C683" s="48"/>
-      <c r="D683" s="48"/>
-      <c r="E683" s="48"/>
-      <c r="F683" s="48"/>
+      <c r="B683" s="56"/>
+      <c r="C683" s="56"/>
+      <c r="D683" s="56"/>
+      <c r="E683" s="56"/>
+      <c r="F683" s="56"/>
       <c r="G683" s="22"/>
       <c r="H683" s="22"/>
     </row>
@@ -8945,8 +8940,8 @@
       <c r="B696" s="25"/>
       <c r="C696" s="28"/>
       <c r="D696" s="28"/>
-      <c r="E696" s="48"/>
-      <c r="F696" s="48"/>
+      <c r="E696" s="56"/>
+      <c r="F696" s="56"/>
       <c r="G696" s="22"/>
       <c r="H696" s="22"/>
     </row>
@@ -9072,11 +9067,11 @@
     </row>
     <row r="709" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A709" s="23"/>
-      <c r="B709" s="48"/>
-      <c r="C709" s="48"/>
+      <c r="B709" s="56"/>
+      <c r="C709" s="56"/>
       <c r="D709" s="28"/>
-      <c r="E709" s="48"/>
-      <c r="F709" s="48"/>
+      <c r="E709" s="56"/>
+      <c r="F709" s="56"/>
       <c r="G709" s="22"/>
       <c r="H709" s="22"/>
     </row>
@@ -9120,6 +9115,7 @@
     <mergeCell ref="B356:F356"/>
     <mergeCell ref="B334:F334"/>
     <mergeCell ref="B349:F349"/>
+    <mergeCell ref="C290:F290"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="D22:E22"/>
@@ -9133,6 +9129,7 @@
     <mergeCell ref="E40:F40"/>
     <mergeCell ref="E41:F41"/>
     <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B34:F34"/>
     <mergeCell ref="B44:D44"/>
     <mergeCell ref="B527:F527"/>
     <mergeCell ref="B540:F540"/>
@@ -9144,17 +9141,6 @@
     <mergeCell ref="B501:F501"/>
     <mergeCell ref="B514:F514"/>
     <mergeCell ref="C488:F488"/>
-    <mergeCell ref="B657:F657"/>
-    <mergeCell ref="B670:F670"/>
-    <mergeCell ref="B683:F683"/>
-    <mergeCell ref="B709:C709"/>
-    <mergeCell ref="E709:F709"/>
-    <mergeCell ref="E696:F696"/>
-    <mergeCell ref="B592:F592"/>
-    <mergeCell ref="B605:F605"/>
-    <mergeCell ref="B618:F618"/>
-    <mergeCell ref="B631:F631"/>
-    <mergeCell ref="B644:D644"/>
     <mergeCell ref="B262:F262"/>
     <mergeCell ref="B263:F263"/>
     <mergeCell ref="B268:F268"/>
@@ -9168,6 +9154,17 @@
     <mergeCell ref="B219:F219"/>
     <mergeCell ref="B159:E159"/>
     <mergeCell ref="B162:E162"/>
+    <mergeCell ref="B657:F657"/>
+    <mergeCell ref="B670:F670"/>
+    <mergeCell ref="B683:F683"/>
+    <mergeCell ref="B709:C709"/>
+    <mergeCell ref="E709:F709"/>
+    <mergeCell ref="E696:F696"/>
+    <mergeCell ref="B592:F592"/>
+    <mergeCell ref="B605:F605"/>
+    <mergeCell ref="B618:F618"/>
+    <mergeCell ref="B631:F631"/>
+    <mergeCell ref="B644:D644"/>
     <mergeCell ref="B179:F179"/>
     <mergeCell ref="B222:F222"/>
     <mergeCell ref="B228:F228"/>
@@ -9185,6 +9182,13 @@
     <mergeCell ref="B332:F332"/>
     <mergeCell ref="B333:F333"/>
     <mergeCell ref="B338:F338"/>
+    <mergeCell ref="C298:F298"/>
+    <mergeCell ref="B312:F312"/>
+    <mergeCell ref="B254:F254"/>
+    <mergeCell ref="B252:F252"/>
+    <mergeCell ref="B253:F253"/>
+    <mergeCell ref="B305:F305"/>
+    <mergeCell ref="B304:F304"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="D14:F14"/>
@@ -9238,14 +9242,10 @@
     <mergeCell ref="B171:F171"/>
     <mergeCell ref="B160:E160"/>
     <mergeCell ref="B161:E161"/>
-    <mergeCell ref="C298:F298"/>
-    <mergeCell ref="B312:F312"/>
-    <mergeCell ref="B254:F254"/>
-    <mergeCell ref="B252:F252"/>
-    <mergeCell ref="B253:F253"/>
-    <mergeCell ref="B305:F305"/>
-    <mergeCell ref="B304:F304"/>
-    <mergeCell ref="C290:F290"/>
+    <mergeCell ref="B141:F141"/>
+    <mergeCell ref="B146:F146"/>
+    <mergeCell ref="B140:F140"/>
+    <mergeCell ref="C65:F65"/>
     <mergeCell ref="C291:F291"/>
     <mergeCell ref="C296:F296"/>
     <mergeCell ref="C294:F294"/>
@@ -9284,10 +9284,6 @@
     <mergeCell ref="B172:F172"/>
     <mergeCell ref="B180:F180"/>
     <mergeCell ref="B138:F138"/>
-    <mergeCell ref="B141:F141"/>
-    <mergeCell ref="B146:F146"/>
-    <mergeCell ref="B140:F140"/>
-    <mergeCell ref="C65:F65"/>
     <mergeCell ref="B87:F87"/>
     <mergeCell ref="B74:F74"/>
     <mergeCell ref="B61:F61"/>
@@ -9310,7 +9306,6 @@
     <mergeCell ref="B102:F102"/>
     <mergeCell ref="B81:F81"/>
     <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B34:F34"/>
     <mergeCell ref="B79:F79"/>
     <mergeCell ref="B73:F73"/>
     <mergeCell ref="B75:F75"/>
@@ -9331,226 +9326,4 @@
   <pageSetup scale="45" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C52AC05ABFE72848B064B29BAAE56978" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e46e943270ee26bd29fcd296d6dc0391">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d7f988bb-f583-49a7-b3d9-d97123f42079" xmlns:ns3="3edb9f2a-be93-48b2-8353-85a0a13fb21f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="500a4c8be8b02aa6735dedf3aecdc3bf" ns2:_="" ns3:_="">
-    <xsd:import namespace="d7f988bb-f583-49a7-b3d9-d97123f42079"/>
-    <xsd:import namespace="3edb9f2a-be93-48b2-8353-85a0a13fb21f"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d7f988bb-f583-49a7-b3d9-d97123f42079" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="10" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="3edb9f2a-be93-48b2-8353-85a0a13fb21f" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="11" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="12" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1294CE1-7D2C-4304-B992-670D67B17C6E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D80FE525-8B83-4691-86E0-0CA5EFF1F83B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03D1DCC7-5662-4D3A-BFAB-AD438884EE5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d7f988bb-f583-49a7-b3d9-d97123f42079"/>
-    <ds:schemaRef ds:uri="3edb9f2a-be93-48b2-8353-85a0a13fb21f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>